<commit_message>
Agrega datos actualizados para grafica1 y grafica2 de asegurados
</commit_message>
<xml_diff>
--- a/data/asegurados_graph1.xlsx
+++ b/data/asegurados_graph1.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="308" uniqueCount="308">
   <si>
     <t>date_df</t>
   </si>
@@ -23,6 +23,726 @@
   </si>
   <si>
     <t>variacion</t>
+  </si>
+  <si>
+    <t>2000-01-31</t>
+  </si>
+  <si>
+    <t>2000-02-29</t>
+  </si>
+  <si>
+    <t>2000-03-31</t>
+  </si>
+  <si>
+    <t>2000-04-30</t>
+  </si>
+  <si>
+    <t>2000-05-31</t>
+  </si>
+  <si>
+    <t>2000-06-30</t>
+  </si>
+  <si>
+    <t>2000-07-31</t>
+  </si>
+  <si>
+    <t>2000-08-31</t>
+  </si>
+  <si>
+    <t>2000-09-30</t>
+  </si>
+  <si>
+    <t>2000-10-31</t>
+  </si>
+  <si>
+    <t>2000-11-30</t>
+  </si>
+  <si>
+    <t>2000-12-31</t>
+  </si>
+  <si>
+    <t>2001-01-31</t>
+  </si>
+  <si>
+    <t>2001-02-28</t>
+  </si>
+  <si>
+    <t>2001-03-31</t>
+  </si>
+  <si>
+    <t>2001-04-30</t>
+  </si>
+  <si>
+    <t>2001-05-31</t>
+  </si>
+  <si>
+    <t>2001-06-30</t>
+  </si>
+  <si>
+    <t>2001-07-31</t>
+  </si>
+  <si>
+    <t>2001-08-31</t>
+  </si>
+  <si>
+    <t>2001-09-30</t>
+  </si>
+  <si>
+    <t>2001-10-31</t>
+  </si>
+  <si>
+    <t>2001-11-30</t>
+  </si>
+  <si>
+    <t>2001-12-31</t>
+  </si>
+  <si>
+    <t>2002-01-31</t>
+  </si>
+  <si>
+    <t>2002-02-28</t>
+  </si>
+  <si>
+    <t>2002-03-31</t>
+  </si>
+  <si>
+    <t>2002-04-30</t>
+  </si>
+  <si>
+    <t>2002-05-31</t>
+  </si>
+  <si>
+    <t>2002-06-30</t>
+  </si>
+  <si>
+    <t>2002-07-31</t>
+  </si>
+  <si>
+    <t>2002-08-31</t>
+  </si>
+  <si>
+    <t>2002-09-30</t>
+  </si>
+  <si>
+    <t>2002-10-31</t>
+  </si>
+  <si>
+    <t>2002-11-30</t>
+  </si>
+  <si>
+    <t>2002-12-31</t>
+  </si>
+  <si>
+    <t>2003-01-31</t>
+  </si>
+  <si>
+    <t>2003-02-28</t>
+  </si>
+  <si>
+    <t>2003-03-31</t>
+  </si>
+  <si>
+    <t>2003-04-30</t>
+  </si>
+  <si>
+    <t>2003-05-31</t>
+  </si>
+  <si>
+    <t>2003-06-30</t>
+  </si>
+  <si>
+    <t>2003-07-31</t>
+  </si>
+  <si>
+    <t>2003-08-31</t>
+  </si>
+  <si>
+    <t>2003-09-30</t>
+  </si>
+  <si>
+    <t>2003-10-31</t>
+  </si>
+  <si>
+    <t>2003-11-30</t>
+  </si>
+  <si>
+    <t>2003-12-31</t>
+  </si>
+  <si>
+    <t>2004-01-31</t>
+  </si>
+  <si>
+    <t>2004-02-29</t>
+  </si>
+  <si>
+    <t>2004-03-31</t>
+  </si>
+  <si>
+    <t>2004-04-30</t>
+  </si>
+  <si>
+    <t>2004-05-31</t>
+  </si>
+  <si>
+    <t>2004-06-30</t>
+  </si>
+  <si>
+    <t>2004-07-31</t>
+  </si>
+  <si>
+    <t>2004-08-31</t>
+  </si>
+  <si>
+    <t>2004-09-30</t>
+  </si>
+  <si>
+    <t>2004-10-31</t>
+  </si>
+  <si>
+    <t>2004-11-30</t>
+  </si>
+  <si>
+    <t>2004-12-31</t>
+  </si>
+  <si>
+    <t>2005-01-31</t>
+  </si>
+  <si>
+    <t>2005-02-28</t>
+  </si>
+  <si>
+    <t>2005-03-31</t>
+  </si>
+  <si>
+    <t>2005-04-30</t>
+  </si>
+  <si>
+    <t>2005-05-31</t>
+  </si>
+  <si>
+    <t>2005-06-30</t>
+  </si>
+  <si>
+    <t>2005-07-31</t>
+  </si>
+  <si>
+    <t>2005-08-31</t>
+  </si>
+  <si>
+    <t>2005-09-30</t>
+  </si>
+  <si>
+    <t>2005-10-31</t>
+  </si>
+  <si>
+    <t>2005-11-30</t>
+  </si>
+  <si>
+    <t>2005-12-31</t>
+  </si>
+  <si>
+    <t>2006-01-31</t>
+  </si>
+  <si>
+    <t>2006-02-28</t>
+  </si>
+  <si>
+    <t>2006-03-31</t>
+  </si>
+  <si>
+    <t>2006-04-30</t>
+  </si>
+  <si>
+    <t>2006-05-31</t>
+  </si>
+  <si>
+    <t>2006-06-30</t>
+  </si>
+  <si>
+    <t>2006-07-31</t>
+  </si>
+  <si>
+    <t>2006-08-31</t>
+  </si>
+  <si>
+    <t>2006-09-30</t>
+  </si>
+  <si>
+    <t>2006-10-31</t>
+  </si>
+  <si>
+    <t>2006-11-30</t>
+  </si>
+  <si>
+    <t>2006-12-31</t>
+  </si>
+  <si>
+    <t>2007-01-31</t>
+  </si>
+  <si>
+    <t>2007-02-28</t>
+  </si>
+  <si>
+    <t>2007-03-31</t>
+  </si>
+  <si>
+    <t>2007-04-30</t>
+  </si>
+  <si>
+    <t>2007-05-31</t>
+  </si>
+  <si>
+    <t>2007-06-30</t>
+  </si>
+  <si>
+    <t>2007-07-31</t>
+  </si>
+  <si>
+    <t>2007-08-31</t>
+  </si>
+  <si>
+    <t>2007-09-30</t>
+  </si>
+  <si>
+    <t>2007-10-31</t>
+  </si>
+  <si>
+    <t>2007-11-30</t>
+  </si>
+  <si>
+    <t>2007-12-31</t>
+  </si>
+  <si>
+    <t>2008-01-31</t>
+  </si>
+  <si>
+    <t>2008-02-29</t>
+  </si>
+  <si>
+    <t>2008-03-31</t>
+  </si>
+  <si>
+    <t>2008-04-30</t>
+  </si>
+  <si>
+    <t>2008-05-31</t>
+  </si>
+  <si>
+    <t>2008-06-30</t>
+  </si>
+  <si>
+    <t>2008-07-31</t>
+  </si>
+  <si>
+    <t>2008-08-31</t>
+  </si>
+  <si>
+    <t>2008-09-30</t>
+  </si>
+  <si>
+    <t>2008-10-31</t>
+  </si>
+  <si>
+    <t>2008-11-30</t>
+  </si>
+  <si>
+    <t>2008-12-31</t>
+  </si>
+  <si>
+    <t>2009-01-31</t>
+  </si>
+  <si>
+    <t>2009-02-28</t>
+  </si>
+  <si>
+    <t>2009-03-31</t>
+  </si>
+  <si>
+    <t>2009-04-30</t>
+  </si>
+  <si>
+    <t>2009-05-31</t>
+  </si>
+  <si>
+    <t>2009-06-30</t>
+  </si>
+  <si>
+    <t>2009-07-31</t>
+  </si>
+  <si>
+    <t>2009-08-31</t>
+  </si>
+  <si>
+    <t>2009-09-30</t>
+  </si>
+  <si>
+    <t>2009-10-31</t>
+  </si>
+  <si>
+    <t>2009-11-30</t>
+  </si>
+  <si>
+    <t>2009-12-31</t>
+  </si>
+  <si>
+    <t>2010-01-31</t>
+  </si>
+  <si>
+    <t>2010-02-29</t>
+  </si>
+  <si>
+    <t>2010-03-31</t>
+  </si>
+  <si>
+    <t>2010-04-30</t>
+  </si>
+  <si>
+    <t>2010-05-31</t>
+  </si>
+  <si>
+    <t>2010-06-30</t>
+  </si>
+  <si>
+    <t>2010-07-31</t>
+  </si>
+  <si>
+    <t>2010-08-31</t>
+  </si>
+  <si>
+    <t>2010-09-30</t>
+  </si>
+  <si>
+    <t>2010-10-31</t>
+  </si>
+  <si>
+    <t>2010-11-30</t>
+  </si>
+  <si>
+    <t>2010-12-31</t>
+  </si>
+  <si>
+    <t>2011-01-31</t>
+  </si>
+  <si>
+    <t>2011-02-29</t>
+  </si>
+  <si>
+    <t>2011-03-31</t>
+  </si>
+  <si>
+    <t>2011-04-30</t>
+  </si>
+  <si>
+    <t>2011-05-31</t>
+  </si>
+  <si>
+    <t>2011-06-30</t>
+  </si>
+  <si>
+    <t>2011-07-31</t>
+  </si>
+  <si>
+    <t>2011-08-31</t>
+  </si>
+  <si>
+    <t>2011-09-30</t>
+  </si>
+  <si>
+    <t>2011-10-31</t>
+  </si>
+  <si>
+    <t>2011-11-30</t>
+  </si>
+  <si>
+    <t>2011-12-31</t>
+  </si>
+  <si>
+    <t>2012-01-31</t>
+  </si>
+  <si>
+    <t>2012-02-29</t>
+  </si>
+  <si>
+    <t>2012-03-31</t>
+  </si>
+  <si>
+    <t>2012-04-30</t>
+  </si>
+  <si>
+    <t>2012-05-31</t>
+  </si>
+  <si>
+    <t>2012-06-30</t>
+  </si>
+  <si>
+    <t>2012-07-31</t>
+  </si>
+  <si>
+    <t>2012-08-31</t>
+  </si>
+  <si>
+    <t>2012-09-30</t>
+  </si>
+  <si>
+    <t>2012-10-31</t>
+  </si>
+  <si>
+    <t>2012-11-30</t>
+  </si>
+  <si>
+    <t>2012-12-31</t>
+  </si>
+  <si>
+    <t>2013-01-31</t>
+  </si>
+  <si>
+    <t>2013-02-28</t>
+  </si>
+  <si>
+    <t>2013-03-31</t>
+  </si>
+  <si>
+    <t>2013-04-30</t>
+  </si>
+  <si>
+    <t>2013-05-31</t>
+  </si>
+  <si>
+    <t>2013-06-30</t>
+  </si>
+  <si>
+    <t>2013-07-31</t>
+  </si>
+  <si>
+    <t>2013-08-31</t>
+  </si>
+  <si>
+    <t>2013-09-30</t>
+  </si>
+  <si>
+    <t>2013-10-31</t>
+  </si>
+  <si>
+    <t>2013-11-30</t>
+  </si>
+  <si>
+    <t>2013-12-31</t>
+  </si>
+  <si>
+    <t>2014-01-31</t>
+  </si>
+  <si>
+    <t>2014-02-28</t>
+  </si>
+  <si>
+    <t>2014-03-31</t>
+  </si>
+  <si>
+    <t>2014-04-30</t>
+  </si>
+  <si>
+    <t>2014-05-31</t>
+  </si>
+  <si>
+    <t>2014-06-30</t>
+  </si>
+  <si>
+    <t>2014-07-31</t>
+  </si>
+  <si>
+    <t>2014-08-31</t>
+  </si>
+  <si>
+    <t>2014-09-30</t>
+  </si>
+  <si>
+    <t>2014-10-31</t>
+  </si>
+  <si>
+    <t>2014-11-30</t>
+  </si>
+  <si>
+    <t>2014-12-31</t>
+  </si>
+  <si>
+    <t>2015-01-31</t>
+  </si>
+  <si>
+    <t>2015-02-28</t>
+  </si>
+  <si>
+    <t>2015-03-31</t>
+  </si>
+  <si>
+    <t>2015-04-30</t>
+  </si>
+  <si>
+    <t>2015-05-31</t>
+  </si>
+  <si>
+    <t>2015-06-30</t>
+  </si>
+  <si>
+    <t>2015-07-31</t>
+  </si>
+  <si>
+    <t>2015-08-31</t>
+  </si>
+  <si>
+    <t>2015-09-30</t>
+  </si>
+  <si>
+    <t>2015-10-31</t>
+  </si>
+  <si>
+    <t>2015-11-30</t>
+  </si>
+  <si>
+    <t>2015-12-31</t>
+  </si>
+  <si>
+    <t>2016-01-31</t>
+  </si>
+  <si>
+    <t>2016-02-29</t>
+  </si>
+  <si>
+    <t>2016-03-31</t>
+  </si>
+  <si>
+    <t>2016-04-30</t>
+  </si>
+  <si>
+    <t>2016-05-31</t>
+  </si>
+  <si>
+    <t>2016-06-30</t>
+  </si>
+  <si>
+    <t>2016-07-31</t>
+  </si>
+  <si>
+    <t>2016-08-31</t>
+  </si>
+  <si>
+    <t>2016-09-30</t>
+  </si>
+  <si>
+    <t>2016-10-31</t>
+  </si>
+  <si>
+    <t>2016-11-30</t>
+  </si>
+  <si>
+    <t>2016-12-31</t>
+  </si>
+  <si>
+    <t>2017-01-31</t>
+  </si>
+  <si>
+    <t>2017-02-28</t>
+  </si>
+  <si>
+    <t>2017-03-31</t>
+  </si>
+  <si>
+    <t>2017-04-30</t>
+  </si>
+  <si>
+    <t>2017-05-31</t>
+  </si>
+  <si>
+    <t>2017-06-30</t>
+  </si>
+  <si>
+    <t>2017-07-31</t>
+  </si>
+  <si>
+    <t>2017-08-31</t>
+  </si>
+  <si>
+    <t>2017-09-30</t>
+  </si>
+  <si>
+    <t>2017-10-31</t>
+  </si>
+  <si>
+    <t>2017-11-30</t>
+  </si>
+  <si>
+    <t>2017-12-31</t>
+  </si>
+  <si>
+    <t>2018-01-31</t>
+  </si>
+  <si>
+    <t>2018-02-28</t>
+  </si>
+  <si>
+    <t>2018-03-31</t>
+  </si>
+  <si>
+    <t>2018-04-30</t>
+  </si>
+  <si>
+    <t>2018-05-31</t>
+  </si>
+  <si>
+    <t>2018-06-30</t>
+  </si>
+  <si>
+    <t>2018-07-31</t>
+  </si>
+  <si>
+    <t>2018-08-31</t>
+  </si>
+  <si>
+    <t>2018-09-30</t>
+  </si>
+  <si>
+    <t>2018-10-31</t>
+  </si>
+  <si>
+    <t>2018-11-30</t>
+  </si>
+  <si>
+    <t>2018-12-31</t>
+  </si>
+  <si>
+    <t>2019-01-31</t>
+  </si>
+  <si>
+    <t>2019-02-28</t>
+  </si>
+  <si>
+    <t>2019-03-31</t>
+  </si>
+  <si>
+    <t>2019-04-30</t>
+  </si>
+  <si>
+    <t>2019-05-31</t>
+  </si>
+  <si>
+    <t>2019-06-30</t>
+  </si>
+  <si>
+    <t>2019-07-31</t>
+  </si>
+  <si>
+    <t>2019-08-31</t>
+  </si>
+  <si>
+    <t>2019-09-30</t>
+  </si>
+  <si>
+    <t>2019-10-31</t>
+  </si>
+  <si>
+    <t>2019-11-30</t>
+  </si>
+  <si>
+    <t>2019-12-31</t>
   </si>
   <si>
     <t>2020-01-31</t>
@@ -575,7 +1295,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D66"/>
+  <dimension ref="A1:D306"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -600,7 +1320,7 @@
         <v>3</v>
       </c>
       <c r="C2">
-        <v>20490397</v>
+        <v>12034095</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -611,7 +1331,7 @@
         <v>4</v>
       </c>
       <c r="C3">
-        <v>20613536</v>
+        <v>12158433</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -622,7 +1342,7 @@
         <v>5</v>
       </c>
       <c r="C4">
-        <v>20482943</v>
+        <v>12258841</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -633,7 +1353,7 @@
         <v>6</v>
       </c>
       <c r="C5">
-        <v>19927696</v>
+        <v>12254009</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -644,7 +1364,7 @@
         <v>7</v>
       </c>
       <c r="C6">
-        <v>19583170</v>
+        <v>12345063</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -655,7 +1375,7 @@
         <v>8</v>
       </c>
       <c r="C7">
-        <v>19499859</v>
+        <v>12405558</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -666,7 +1386,7 @@
         <v>9</v>
       </c>
       <c r="C8">
-        <v>19495952</v>
+        <v>12494633</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -677,7 +1397,7 @@
         <v>10</v>
       </c>
       <c r="C9">
-        <v>19588342</v>
+        <v>12554723</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -688,7 +1408,7 @@
         <v>11</v>
       </c>
       <c r="C10">
-        <v>19702192</v>
+        <v>12605656</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -699,7 +1419,7 @@
         <v>12</v>
       </c>
       <c r="C11">
-        <v>19902833</v>
+        <v>12724493</v>
       </c>
     </row>
     <row r="12" spans="1:4">
@@ -710,7 +1430,7 @@
         <v>13</v>
       </c>
       <c r="C12">
-        <v>20051552</v>
+        <v>12777514</v>
       </c>
     </row>
     <row r="13" spans="1:4">
@@ -721,7 +1441,7 @@
         <v>14</v>
       </c>
       <c r="C13">
-        <v>19773732</v>
+        <v>12437760</v>
       </c>
     </row>
     <row r="14" spans="1:4">
@@ -732,10 +1452,10 @@
         <v>15</v>
       </c>
       <c r="C14">
-        <v>19821651</v>
+        <v>12525949</v>
       </c>
       <c r="D14">
-        <v>-3.26</v>
+        <v>4.09</v>
       </c>
     </row>
     <row r="15" spans="1:4">
@@ -746,10 +1466,10 @@
         <v>16</v>
       </c>
       <c r="C15">
-        <v>19936938</v>
+        <v>12559358</v>
       </c>
       <c r="D15">
-        <v>-3.28</v>
+        <v>3.3</v>
       </c>
     </row>
     <row r="16" spans="1:4">
@@ -760,10 +1480,10 @@
         <v>17</v>
       </c>
       <c r="C16">
-        <v>20025709</v>
+        <v>12530250</v>
       </c>
       <c r="D16">
-        <v>-2.23</v>
+        <v>2.21</v>
       </c>
     </row>
     <row r="17" spans="1:4">
@@ -774,10 +1494,10 @@
         <v>18</v>
       </c>
       <c r="C17">
-        <v>20070483</v>
+        <v>12534173</v>
       </c>
       <c r="D17">
-        <v>0.72</v>
+        <v>2.29</v>
       </c>
     </row>
     <row r="18" spans="1:4">
@@ -788,10 +1508,10 @@
         <v>19</v>
       </c>
       <c r="C18">
-        <v>20109444</v>
+        <v>12505105</v>
       </c>
       <c r="D18">
-        <v>2.69</v>
+        <v>1.3</v>
       </c>
     </row>
     <row r="19" spans="1:4">
@@ -802,10 +1522,10 @@
         <v>20</v>
       </c>
       <c r="C19">
-        <v>20175380</v>
+        <v>12418906</v>
       </c>
       <c r="D19">
-        <v>3.46</v>
+        <v>0.11</v>
       </c>
     </row>
     <row r="20" spans="1:4">
@@ -816,10 +1536,10 @@
         <v>21</v>
       </c>
       <c r="C20">
-        <v>20291923</v>
+        <v>12416576</v>
       </c>
       <c r="D20">
-        <v>4.08</v>
+        <v>-0.62</v>
       </c>
     </row>
     <row r="21" spans="1:4">
@@ -830,10 +1550,10 @@
         <v>22</v>
       </c>
       <c r="C21">
-        <v>20420823</v>
+        <v>12406096</v>
       </c>
       <c r="D21">
-        <v>4.25</v>
+        <v>-1.18</v>
       </c>
     </row>
     <row r="22" spans="1:4">
@@ -844,10 +1564,10 @@
         <v>23</v>
       </c>
       <c r="C22">
-        <v>20594919</v>
+        <v>12358665</v>
       </c>
       <c r="D22">
-        <v>4.53</v>
+        <v>-1.96</v>
       </c>
     </row>
     <row r="23" spans="1:4">
@@ -858,10 +1578,10 @@
         <v>24</v>
       </c>
       <c r="C23">
-        <v>20767587</v>
+        <v>12423519</v>
       </c>
       <c r="D23">
-        <v>4.34</v>
+        <v>-2.37</v>
       </c>
     </row>
     <row r="24" spans="1:4">
@@ -872,10 +1592,10 @@
         <v>25</v>
       </c>
       <c r="C24">
-        <v>20933050</v>
+        <v>12451466</v>
       </c>
       <c r="D24">
-        <v>4.4</v>
+        <v>-2.55</v>
       </c>
     </row>
     <row r="25" spans="1:4">
@@ -886,10 +1606,10 @@
         <v>26</v>
       </c>
       <c r="C25">
-        <v>20620148</v>
+        <v>12170945</v>
       </c>
       <c r="D25">
-        <v>4.28</v>
+        <v>-2.15</v>
       </c>
     </row>
     <row r="26" spans="1:4">
@@ -900,10 +1620,10 @@
         <v>27</v>
       </c>
       <c r="C26">
-        <v>20762419</v>
+        <v>12195513</v>
       </c>
       <c r="D26">
-        <v>4.75</v>
+        <v>-2.64</v>
       </c>
     </row>
     <row r="27" spans="1:4">
@@ -914,10 +1634,10 @@
         <v>28</v>
       </c>
       <c r="C27">
-        <v>20941286</v>
+        <v>12275211</v>
       </c>
       <c r="D27">
-        <v>5.04</v>
+        <v>-2.26</v>
       </c>
     </row>
     <row r="28" spans="1:4">
@@ -928,10 +1648,10 @@
         <v>29</v>
       </c>
       <c r="C28">
-        <v>21005852</v>
+        <v>12221087</v>
       </c>
       <c r="D28">
-        <v>4.89</v>
+        <v>-2.47</v>
       </c>
     </row>
     <row r="29" spans="1:4">
@@ -942,10 +1662,10 @@
         <v>30</v>
       </c>
       <c r="C29">
-        <v>21011342</v>
+        <v>12352690</v>
       </c>
       <c r="D29">
-        <v>4.69</v>
+        <v>-1.45</v>
       </c>
     </row>
     <row r="30" spans="1:4">
@@ -956,10 +1676,10 @@
         <v>31</v>
       </c>
       <c r="C30">
-        <v>21008487</v>
+        <v>12338063</v>
       </c>
       <c r="D30">
-        <v>4.47</v>
+        <v>-1.34</v>
       </c>
     </row>
     <row r="31" spans="1:4">
@@ -970,10 +1690,10 @@
         <v>32</v>
       </c>
       <c r="C31">
-        <v>21068708</v>
+        <v>12288156</v>
       </c>
       <c r="D31">
-        <v>4.43</v>
+        <v>-1.05</v>
       </c>
     </row>
     <row r="32" spans="1:4">
@@ -984,10 +1704,10 @@
         <v>33</v>
       </c>
       <c r="C32">
-        <v>21079434</v>
+        <v>12368684</v>
       </c>
       <c r="D32">
-        <v>3.88</v>
+        <v>-0.39</v>
       </c>
     </row>
     <row r="33" spans="1:4">
@@ -998,10 +1718,10 @@
         <v>34</v>
       </c>
       <c r="C33">
-        <v>21236866</v>
+        <v>12340462</v>
       </c>
       <c r="D33">
-        <v>4</v>
+        <v>-0.53</v>
       </c>
     </row>
     <row r="34" spans="1:4">
@@ -1012,10 +1732,10 @@
         <v>35</v>
       </c>
       <c r="C34">
-        <v>21409358</v>
+        <v>12400521</v>
       </c>
       <c r="D34">
-        <v>3.95</v>
+        <v>0.34</v>
       </c>
     </row>
     <row r="35" spans="1:4">
@@ -1026,10 +1746,10 @@
         <v>36</v>
       </c>
       <c r="C35">
-        <v>21617326</v>
+        <v>12457620</v>
       </c>
       <c r="D35">
-        <v>4.09</v>
+        <v>0.27</v>
       </c>
     </row>
     <row r="36" spans="1:4">
@@ -1040,10 +1760,10 @@
         <v>37</v>
       </c>
       <c r="C36">
-        <v>21718601</v>
+        <v>12472617</v>
       </c>
       <c r="D36">
-        <v>3.75</v>
+        <v>0.17</v>
       </c>
     </row>
     <row r="37" spans="1:4">
@@ -1054,10 +1774,10 @@
         <v>38</v>
       </c>
       <c r="C37">
-        <v>21372896</v>
+        <v>12232301</v>
       </c>
       <c r="D37">
-        <v>3.65</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="38" spans="1:4">
@@ -1068,10 +1788,10 @@
         <v>39</v>
       </c>
       <c r="C38">
-        <v>21484595</v>
+        <v>12269469</v>
       </c>
       <c r="D38">
-        <v>3.48</v>
+        <v>0.61</v>
       </c>
     </row>
     <row r="39" spans="1:4">
@@ -1082,10 +1802,10 @@
         <v>40</v>
       </c>
       <c r="C39">
-        <v>21660469</v>
+        <v>12321596</v>
       </c>
       <c r="D39">
-        <v>3.43</v>
+        <v>0.38</v>
       </c>
     </row>
     <row r="40" spans="1:4">
@@ -1096,10 +1816,10 @@
         <v>41</v>
       </c>
       <c r="C40">
-        <v>21796280</v>
+        <v>12348257</v>
       </c>
       <c r="D40">
-        <v>3.76</v>
+        <v>1.04</v>
       </c>
     </row>
     <row r="41" spans="1:4">
@@ -1110,10 +1830,10 @@
         <v>42</v>
       </c>
       <c r="C41">
-        <v>21820291</v>
+        <v>12337553</v>
       </c>
       <c r="D41">
-        <v>3.85</v>
+        <v>-0.12</v>
       </c>
     </row>
     <row r="42" spans="1:4">
@@ -1124,10 +1844,10 @@
         <v>43</v>
       </c>
       <c r="C42">
-        <v>21862909</v>
+        <v>12269056</v>
       </c>
       <c r="D42">
-        <v>4.07</v>
+        <v>-0.5600000000000001</v>
       </c>
     </row>
     <row r="43" spans="1:4">
@@ -1138,10 +1858,10 @@
         <v>44</v>
       </c>
       <c r="C43">
-        <v>21887307</v>
+        <v>12270626</v>
       </c>
       <c r="D43">
-        <v>3.89</v>
+        <v>-0.14</v>
       </c>
     </row>
     <row r="44" spans="1:4">
@@ -1152,10 +1872,10 @@
         <v>45</v>
       </c>
       <c r="C44">
-        <v>21885139</v>
+        <v>12270143</v>
       </c>
       <c r="D44">
-        <v>3.82</v>
+        <v>-0.8</v>
       </c>
     </row>
     <row r="45" spans="1:4">
@@ -1166,10 +1886,10 @@
         <v>46</v>
       </c>
       <c r="C45">
-        <v>21996875</v>
+        <v>12229764</v>
       </c>
       <c r="D45">
-        <v>3.58</v>
+        <v>-0.9</v>
       </c>
     </row>
     <row r="46" spans="1:4">
@@ -1180,10 +1900,10 @@
         <v>47</v>
       </c>
       <c r="C46">
-        <v>22129433</v>
+        <v>12323341</v>
       </c>
       <c r="D46">
-        <v>3.36</v>
+        <v>-0.62</v>
       </c>
     </row>
     <row r="47" spans="1:4">
@@ -1194,10 +1914,10 @@
         <v>48</v>
       </c>
       <c r="C47">
-        <v>22302690</v>
+        <v>12427371</v>
       </c>
       <c r="D47">
-        <v>3.17</v>
+        <v>-0.24</v>
       </c>
     </row>
     <row r="48" spans="1:4">
@@ -1208,10 +1928,10 @@
         <v>49</v>
       </c>
       <c r="C48">
-        <v>22409268</v>
+        <v>12462714</v>
       </c>
       <c r="D48">
-        <v>3.18</v>
+        <v>-0.08</v>
       </c>
     </row>
     <row r="49" spans="1:4">
@@ -1222,10 +1942,10 @@
         <v>50</v>
       </c>
       <c r="C49">
-        <v>22024386</v>
+        <v>12257581</v>
       </c>
       <c r="D49">
-        <v>3.05</v>
+        <v>0.21</v>
       </c>
     </row>
     <row r="50" spans="1:4">
@@ -1236,10 +1956,10 @@
         <v>51</v>
       </c>
       <c r="C50">
-        <v>22133407</v>
+        <v>12294000</v>
       </c>
       <c r="D50">
-        <v>3.02</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="51" spans="1:4">
@@ -1250,10 +1970,10 @@
         <v>52</v>
       </c>
       <c r="C51">
-        <v>22289810</v>
+        <v>12351665</v>
       </c>
       <c r="D51">
-        <v>2.91</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="52" spans="1:4">
@@ -1264,10 +1984,10 @@
         <v>53</v>
       </c>
       <c r="C52">
-        <v>22289345</v>
+        <v>12478529</v>
       </c>
       <c r="D52">
-        <v>2.26</v>
+        <v>1.05</v>
       </c>
     </row>
     <row r="53" spans="1:4">
@@ -1278,10 +1998,10 @@
         <v>54</v>
       </c>
       <c r="C53">
-        <v>22374202</v>
+        <v>12505272</v>
       </c>
       <c r="D53">
-        <v>2.54</v>
+        <v>1.36</v>
       </c>
     </row>
     <row r="54" spans="1:4">
@@ -1292,10 +2012,10 @@
         <v>55</v>
       </c>
       <c r="C54">
-        <v>22348999</v>
+        <v>12495167</v>
       </c>
       <c r="D54">
-        <v>2.22</v>
+        <v>1.84</v>
       </c>
     </row>
     <row r="55" spans="1:4">
@@ -1306,10 +2026,10 @@
         <v>56</v>
       </c>
       <c r="C55">
-        <v>22319444</v>
+        <v>12515338</v>
       </c>
       <c r="D55">
-        <v>1.97</v>
+        <v>1.99</v>
       </c>
     </row>
     <row r="56" spans="1:4">
@@ -1320,10 +2040,10 @@
         <v>57</v>
       </c>
       <c r="C56">
-        <v>22331788</v>
+        <v>12550854</v>
       </c>
       <c r="D56">
-        <v>2.04</v>
+        <v>2.29</v>
       </c>
     </row>
     <row r="57" spans="1:4">
@@ -1334,10 +2054,10 @@
         <v>58</v>
       </c>
       <c r="C57">
-        <v>22389835</v>
+        <v>12597254</v>
       </c>
       <c r="D57">
-        <v>1.79</v>
+        <v>3</v>
       </c>
     </row>
     <row r="58" spans="1:4">
@@ -1348,10 +2068,10 @@
         <v>59</v>
       </c>
       <c r="C58">
-        <v>22480803</v>
+        <v>12683727</v>
       </c>
       <c r="D58">
-        <v>1.59</v>
+        <v>2.92</v>
       </c>
     </row>
     <row r="59" spans="1:4">
@@ -1362,10 +2082,10 @@
         <v>60</v>
       </c>
       <c r="C59">
-        <v>22618942</v>
+        <v>12737398</v>
       </c>
       <c r="D59">
-        <v>1.42</v>
+        <v>2.49</v>
       </c>
     </row>
     <row r="60" spans="1:4">
@@ -1376,10 +2096,10 @@
         <v>61</v>
       </c>
       <c r="C60">
-        <v>22643638</v>
+        <v>12871388</v>
       </c>
       <c r="D60">
-        <v>1.05</v>
+        <v>3.28</v>
       </c>
     </row>
     <row r="61" spans="1:4">
@@ -1390,10 +2110,10 @@
         <v>62</v>
       </c>
       <c r="C61">
-        <v>22238379</v>
+        <v>12632877</v>
       </c>
       <c r="D61">
-        <v>0.97</v>
+        <v>3.06</v>
       </c>
     </row>
     <row r="62" spans="1:4">
@@ -1404,10 +2124,10 @@
         <v>63</v>
       </c>
       <c r="C62">
-        <v>22311546</v>
+        <v>12697125</v>
       </c>
       <c r="D62">
-        <v>0.8</v>
+        <v>3.28</v>
       </c>
     </row>
     <row r="63" spans="1:4">
@@ -1418,10 +2138,10 @@
         <v>64</v>
       </c>
       <c r="C63">
-        <v>22430931</v>
+        <v>12788890</v>
       </c>
       <c r="D63">
-        <v>0.63</v>
+        <v>3.54</v>
       </c>
     </row>
     <row r="64" spans="1:4">
@@ -1432,10 +2152,10 @@
         <v>65</v>
       </c>
       <c r="C64">
-        <v>22465110</v>
+        <v>12799019</v>
       </c>
       <c r="D64">
-        <v>0.79</v>
+        <v>2.57</v>
       </c>
     </row>
     <row r="65" spans="1:4">
@@ -1446,10 +2166,10 @@
         <v>66</v>
       </c>
       <c r="C65">
-        <v>22417668</v>
+        <v>12852756</v>
       </c>
       <c r="D65">
-        <v>0.19</v>
+        <v>2.78</v>
       </c>
     </row>
     <row r="66" spans="1:4">
@@ -1460,9 +2180,3369 @@
         <v>67</v>
       </c>
       <c r="C66">
+        <v>12884166</v>
+      </c>
+      <c r="D66">
+        <v>3.11</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4">
+      <c r="A67" s="1">
+        <v>65</v>
+      </c>
+      <c r="B67" t="s">
+        <v>68</v>
+      </c>
+      <c r="C67">
+        <v>12911021</v>
+      </c>
+      <c r="D67">
+        <v>3.16</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4">
+      <c r="A68" s="1">
+        <v>66</v>
+      </c>
+      <c r="B68" t="s">
+        <v>69</v>
+      </c>
+      <c r="C68">
+        <v>12904401</v>
+      </c>
+      <c r="D68">
+        <v>2.82</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4">
+      <c r="A69" s="1">
+        <v>67</v>
+      </c>
+      <c r="B69" t="s">
+        <v>70</v>
+      </c>
+      <c r="C69">
+        <v>13014610</v>
+      </c>
+      <c r="D69">
+        <v>3.31</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4">
+      <c r="A70" s="1">
+        <v>68</v>
+      </c>
+      <c r="B70" t="s">
+        <v>71</v>
+      </c>
+      <c r="C70">
+        <v>13114254</v>
+      </c>
+      <c r="D70">
+        <v>3.39</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4">
+      <c r="A71" s="1">
+        <v>69</v>
+      </c>
+      <c r="B71" t="s">
+        <v>72</v>
+      </c>
+      <c r="C71">
+        <v>13234501</v>
+      </c>
+      <c r="D71">
+        <v>3.9</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4">
+      <c r="A72" s="1">
+        <v>70</v>
+      </c>
+      <c r="B72" t="s">
+        <v>73</v>
+      </c>
+      <c r="C72">
+        <v>13327162</v>
+      </c>
+      <c r="D72">
+        <v>3.54</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4">
+      <c r="A73" s="1">
+        <v>71</v>
+      </c>
+      <c r="B73" t="s">
+        <v>74</v>
+      </c>
+      <c r="C73">
+        <v>13061565</v>
+      </c>
+      <c r="D73">
+        <v>3.39</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4">
+      <c r="A74" s="1">
+        <v>72</v>
+      </c>
+      <c r="B74" t="s">
+        <v>75</v>
+      </c>
+      <c r="C74">
+        <v>13174495</v>
+      </c>
+      <c r="D74">
+        <v>3.76</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4">
+      <c r="A75" s="1">
+        <v>73</v>
+      </c>
+      <c r="B75" t="s">
+        <v>76</v>
+      </c>
+      <c r="C75">
+        <v>13285285</v>
+      </c>
+      <c r="D75">
+        <v>3.88</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4">
+      <c r="A76" s="1">
+        <v>74</v>
+      </c>
+      <c r="B76" t="s">
+        <v>77</v>
+      </c>
+      <c r="C76">
+        <v>13392387</v>
+      </c>
+      <c r="D76">
+        <v>4.64</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4">
+      <c r="A77" s="1">
+        <v>75</v>
+      </c>
+      <c r="B77" t="s">
+        <v>78</v>
+      </c>
+      <c r="C77">
+        <v>13402509</v>
+      </c>
+      <c r="D77">
+        <v>4.28</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4">
+      <c r="A78" s="1">
+        <v>76</v>
+      </c>
+      <c r="B78" t="s">
+        <v>79</v>
+      </c>
+      <c r="C78">
+        <v>13486515</v>
+      </c>
+      <c r="D78">
+        <v>4.68</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4">
+      <c r="A79" s="1">
+        <v>77</v>
+      </c>
+      <c r="B79" t="s">
+        <v>80</v>
+      </c>
+      <c r="C79">
+        <v>13550640</v>
+      </c>
+      <c r="D79">
+        <v>4.95</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4">
+      <c r="A80" s="1">
+        <v>78</v>
+      </c>
+      <c r="B80" t="s">
+        <v>81</v>
+      </c>
+      <c r="C80">
+        <v>13604538</v>
+      </c>
+      <c r="D80">
+        <v>5.43</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4">
+      <c r="A81" s="1">
+        <v>79</v>
+      </c>
+      <c r="B81" t="s">
+        <v>82</v>
+      </c>
+      <c r="C81">
+        <v>13676931</v>
+      </c>
+      <c r="D81">
+        <v>5.09</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4">
+      <c r="A82" s="1">
+        <v>80</v>
+      </c>
+      <c r="B82" t="s">
+        <v>83</v>
+      </c>
+      <c r="C82">
+        <v>13756687</v>
+      </c>
+      <c r="D82">
+        <v>4.9</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4">
+      <c r="A83" s="1">
+        <v>81</v>
+      </c>
+      <c r="B83" t="s">
+        <v>84</v>
+      </c>
+      <c r="C83">
+        <v>13894328</v>
+      </c>
+      <c r="D83">
+        <v>4.99</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4">
+      <c r="A84" s="1">
+        <v>82</v>
+      </c>
+      <c r="B84" t="s">
+        <v>85</v>
+      </c>
+      <c r="C84">
+        <v>13981314</v>
+      </c>
+      <c r="D84">
+        <v>4.91</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4">
+      <c r="A85" s="1">
+        <v>83</v>
+      </c>
+      <c r="B85" t="s">
+        <v>86</v>
+      </c>
+      <c r="C85">
+        <v>13678492</v>
+      </c>
+      <c r="D85">
+        <v>4.72</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4">
+      <c r="A86" s="1">
+        <v>84</v>
+      </c>
+      <c r="B86" t="s">
+        <v>87</v>
+      </c>
+      <c r="C86">
+        <v>13794601</v>
+      </c>
+      <c r="D86">
+        <v>4.71</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4">
+      <c r="A87" s="1">
+        <v>85</v>
+      </c>
+      <c r="B87" t="s">
+        <v>88</v>
+      </c>
+      <c r="C87">
+        <v>13908701</v>
+      </c>
+      <c r="D87">
+        <v>4.69</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4">
+      <c r="A88" s="1">
+        <v>86</v>
+      </c>
+      <c r="B88" t="s">
+        <v>89</v>
+      </c>
+      <c r="C88">
+        <v>13973905</v>
+      </c>
+      <c r="D88">
+        <v>4.34</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4">
+      <c r="A89" s="1">
+        <v>87</v>
+      </c>
+      <c r="B89" t="s">
+        <v>90</v>
+      </c>
+      <c r="C89">
+        <v>14043649</v>
+      </c>
+      <c r="D89">
+        <v>4.78</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4">
+      <c r="A90" s="1">
+        <v>88</v>
+      </c>
+      <c r="B90" t="s">
+        <v>91</v>
+      </c>
+      <c r="C90">
+        <v>14072151</v>
+      </c>
+      <c r="D90">
+        <v>4.34</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4">
+      <c r="A91" s="1">
+        <v>89</v>
+      </c>
+      <c r="B91" t="s">
+        <v>92</v>
+      </c>
+      <c r="C91">
+        <v>14089092</v>
+      </c>
+      <c r="D91">
+        <v>3.97</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4">
+      <c r="A92" s="1">
+        <v>90</v>
+      </c>
+      <c r="B92" t="s">
+        <v>93</v>
+      </c>
+      <c r="C92">
+        <v>14156216</v>
+      </c>
+      <c r="D92">
+        <v>4.06</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4">
+      <c r="A93" s="1">
+        <v>91</v>
+      </c>
+      <c r="B93" t="s">
+        <v>94</v>
+      </c>
+      <c r="C93">
+        <v>14224297</v>
+      </c>
+      <c r="D93">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4">
+      <c r="A94" s="1">
+        <v>92</v>
+      </c>
+      <c r="B94" t="s">
+        <v>95</v>
+      </c>
+      <c r="C94">
+        <v>14283377</v>
+      </c>
+      <c r="D94">
+        <v>3.83</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4">
+      <c r="A95" s="1">
+        <v>93</v>
+      </c>
+      <c r="B95" t="s">
+        <v>96</v>
+      </c>
+      <c r="C95">
+        <v>14441717</v>
+      </c>
+      <c r="D95">
+        <v>3.94</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4">
+      <c r="A96" s="1">
+        <v>94</v>
+      </c>
+      <c r="B96" t="s">
+        <v>97</v>
+      </c>
+      <c r="C96">
+        <v>14539497</v>
+      </c>
+      <c r="D96">
+        <v>3.99</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4">
+      <c r="A97" s="1">
+        <v>95</v>
+      </c>
+      <c r="B97" t="s">
+        <v>98</v>
+      </c>
+      <c r="C97">
+        <v>14207706</v>
+      </c>
+      <c r="D97">
+        <v>3.87</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4">
+      <c r="A98" s="1">
+        <v>96</v>
+      </c>
+      <c r="B98" t="s">
+        <v>99</v>
+      </c>
+      <c r="C98">
+        <v>14315318</v>
+      </c>
+      <c r="D98">
+        <v>3.77</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4">
+      <c r="A99" s="1">
+        <v>97</v>
+      </c>
+      <c r="B99" t="s">
+        <v>100</v>
+      </c>
+      <c r="C99">
+        <v>14396101</v>
+      </c>
+      <c r="D99">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4">
+      <c r="A100" s="1">
+        <v>98</v>
+      </c>
+      <c r="B100" t="s">
+        <v>101</v>
+      </c>
+      <c r="C100">
+        <v>14400376</v>
+      </c>
+      <c r="D100">
+        <v>3.05</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4">
+      <c r="A101" s="1">
+        <v>99</v>
+      </c>
+      <c r="B101" t="s">
+        <v>102</v>
+      </c>
+      <c r="C101">
+        <v>14480066</v>
+      </c>
+      <c r="D101">
+        <v>3.11</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4">
+      <c r="A102" s="1">
+        <v>100</v>
+      </c>
+      <c r="B102" t="s">
+        <v>103</v>
+      </c>
+      <c r="C102">
+        <v>14443848</v>
+      </c>
+      <c r="D102">
+        <v>2.64</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4">
+      <c r="A103" s="1">
+        <v>101</v>
+      </c>
+      <c r="B103" t="s">
+        <v>104</v>
+      </c>
+      <c r="C103">
+        <v>14472908</v>
+      </c>
+      <c r="D103">
+        <v>2.72</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4">
+      <c r="A104" s="1">
+        <v>102</v>
+      </c>
+      <c r="B104" t="s">
+        <v>105</v>
+      </c>
+      <c r="C104">
+        <v>14483011</v>
+      </c>
+      <c r="D104">
+        <v>2.31</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4">
+      <c r="A105" s="1">
+        <v>103</v>
+      </c>
+      <c r="B105" t="s">
+        <v>106</v>
+      </c>
+      <c r="C105">
+        <v>14460993</v>
+      </c>
+      <c r="D105">
+        <v>1.66</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4">
+      <c r="A106" s="1">
+        <v>104</v>
+      </c>
+      <c r="B106" t="s">
+        <v>107</v>
+      </c>
+      <c r="C106">
+        <v>14526347</v>
+      </c>
+      <c r="D106">
+        <v>1.7</v>
+      </c>
+    </row>
+    <row r="107" spans="1:4">
+      <c r="A107" s="1">
+        <v>105</v>
+      </c>
+      <c r="B107" t="s">
+        <v>108</v>
+      </c>
+      <c r="C107">
+        <v>14564570</v>
+      </c>
+      <c r="D107">
+        <v>0.85</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4">
+      <c r="A108" s="1">
+        <v>106</v>
+      </c>
+      <c r="B108" t="s">
+        <v>109</v>
+      </c>
+      <c r="C108">
+        <v>14505253</v>
+      </c>
+      <c r="D108">
+        <v>-0.24</v>
+      </c>
+    </row>
+    <row r="109" spans="1:4">
+      <c r="A109" s="1">
+        <v>107</v>
+      </c>
+      <c r="B109" t="s">
+        <v>110</v>
+      </c>
+      <c r="C109">
+        <v>14178117</v>
+      </c>
+      <c r="D109">
+        <v>-0.21</v>
+      </c>
+    </row>
+    <row r="110" spans="1:4">
+      <c r="A110" s="1">
+        <v>108</v>
+      </c>
+      <c r="B110" t="s">
+        <v>111</v>
+      </c>
+      <c r="C110">
+        <v>14073102</v>
+      </c>
+      <c r="D110">
+        <v>-1.69</v>
+      </c>
+    </row>
+    <row r="111" spans="1:4">
+      <c r="A111" s="1">
+        <v>109</v>
+      </c>
+      <c r="B111" t="s">
+        <v>112</v>
+      </c>
+      <c r="C111">
+        <v>14026501</v>
+      </c>
+      <c r="D111">
+        <v>-2.57</v>
+      </c>
+    </row>
+    <row r="112" spans="1:4">
+      <c r="A112" s="1">
+        <v>110</v>
+      </c>
+      <c r="B112" t="s">
+        <v>113</v>
+      </c>
+      <c r="C112">
+        <v>14039826</v>
+      </c>
+      <c r="D112">
+        <v>-2.5</v>
+      </c>
+    </row>
+    <row r="113" spans="1:4">
+      <c r="A113" s="1">
+        <v>111</v>
+      </c>
+      <c r="B113" t="s">
+        <v>114</v>
+      </c>
+      <c r="C113">
+        <v>13979608</v>
+      </c>
+      <c r="D113">
+        <v>-3.46</v>
+      </c>
+    </row>
+    <row r="114" spans="1:4">
+      <c r="A114" s="1">
+        <v>112</v>
+      </c>
+      <c r="B114" t="s">
+        <v>115</v>
+      </c>
+      <c r="C114">
+        <v>13868132</v>
+      </c>
+      <c r="D114">
+        <v>-3.99</v>
+      </c>
+    </row>
+    <row r="115" spans="1:4">
+      <c r="A115" s="1">
+        <v>113</v>
+      </c>
+      <c r="B115" t="s">
+        <v>116</v>
+      </c>
+      <c r="C115">
+        <v>13871175</v>
+      </c>
+      <c r="D115">
+        <v>-4.16</v>
+      </c>
+    </row>
+    <row r="116" spans="1:4">
+      <c r="A116" s="1">
+        <v>114</v>
+      </c>
+      <c r="B116" t="s">
+        <v>117</v>
+      </c>
+      <c r="C116">
+        <v>13887498</v>
+      </c>
+      <c r="D116">
+        <v>-4.11</v>
+      </c>
+    </row>
+    <row r="117" spans="1:4">
+      <c r="A117" s="1">
+        <v>115</v>
+      </c>
+      <c r="B117" t="s">
+        <v>118</v>
+      </c>
+      <c r="C117">
+        <v>13918843</v>
+      </c>
+      <c r="D117">
+        <v>-3.75</v>
+      </c>
+    </row>
+    <row r="118" spans="1:4">
+      <c r="A118" s="1">
+        <v>116</v>
+      </c>
+      <c r="B118" t="s">
+        <v>119</v>
+      </c>
+      <c r="C118">
+        <v>13992494</v>
+      </c>
+      <c r="D118">
+        <v>-3.68</v>
+      </c>
+    </row>
+    <row r="119" spans="1:4">
+      <c r="A119" s="1">
+        <v>117</v>
+      </c>
+      <c r="B119" t="s">
+        <v>120</v>
+      </c>
+      <c r="C119">
+        <v>14073749</v>
+      </c>
+      <c r="D119">
+        <v>-3.37</v>
+      </c>
+    </row>
+    <row r="120" spans="1:4">
+      <c r="A120" s="1">
+        <v>118</v>
+      </c>
+      <c r="B120" t="s">
+        <v>121</v>
+      </c>
+      <c r="C120">
+        <v>14192197</v>
+      </c>
+      <c r="D120">
+        <v>-2.16</v>
+      </c>
+    </row>
+    <row r="121" spans="1:4">
+      <c r="A121" s="1">
+        <v>119</v>
+      </c>
+      <c r="B121" t="s">
+        <v>122</v>
+      </c>
+      <c r="C121">
+        <v>14006404</v>
+      </c>
+      <c r="D121">
+        <v>-1.21</v>
+      </c>
+    </row>
+    <row r="122" spans="1:4">
+      <c r="A122" s="1">
+        <v>120</v>
+      </c>
+      <c r="B122" t="s">
+        <v>123</v>
+      </c>
+      <c r="C122">
+        <v>14076279</v>
+      </c>
+      <c r="D122">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="123" spans="1:4">
+      <c r="A123" s="1">
+        <v>121</v>
+      </c>
+      <c r="B123" t="s">
+        <v>124</v>
+      </c>
+      <c r="C123">
+        <v>14204647</v>
+      </c>
+      <c r="D123">
+        <v>1.27</v>
+      </c>
+    </row>
+    <row r="124" spans="1:4">
+      <c r="A124" s="1">
+        <v>122</v>
+      </c>
+      <c r="B124" t="s">
+        <v>125</v>
+      </c>
+      <c r="C124">
+        <v>14341056</v>
+      </c>
+      <c r="D124">
+        <v>2.15</v>
+      </c>
+    </row>
+    <row r="125" spans="1:4">
+      <c r="A125" s="1">
+        <v>123</v>
+      </c>
+      <c r="B125" t="s">
+        <v>126</v>
+      </c>
+      <c r="C125">
+        <v>14408942</v>
+      </c>
+      <c r="D125">
+        <v>3.07</v>
+      </c>
+    </row>
+    <row r="126" spans="1:4">
+      <c r="A126" s="1">
+        <v>124</v>
+      </c>
+      <c r="B126" t="s">
+        <v>127</v>
+      </c>
+      <c r="C126">
+        <v>14433952</v>
+      </c>
+      <c r="D126">
+        <v>4.08</v>
+      </c>
+    </row>
+    <row r="127" spans="1:4">
+      <c r="A127" s="1">
+        <v>125</v>
+      </c>
+      <c r="B127" t="s">
+        <v>128</v>
+      </c>
+      <c r="C127">
+        <v>14480255</v>
+      </c>
+      <c r="D127">
+        <v>4.39</v>
+      </c>
+    </row>
+    <row r="128" spans="1:4">
+      <c r="A128" s="1">
+        <v>126</v>
+      </c>
+      <c r="B128" t="s">
+        <v>129</v>
+      </c>
+      <c r="C128">
+        <v>14518395</v>
+      </c>
+      <c r="D128">
+        <v>4.54</v>
+      </c>
+    </row>
+    <row r="129" spans="1:4">
+      <c r="A129" s="1">
+        <v>127</v>
+      </c>
+      <c r="B129" t="s">
+        <v>130</v>
+      </c>
+      <c r="C129">
+        <v>14593979</v>
+      </c>
+      <c r="D129">
+        <v>4.85</v>
+      </c>
+    </row>
+    <row r="130" spans="1:4">
+      <c r="A130" s="1">
+        <v>128</v>
+      </c>
+      <c r="B130" t="s">
+        <v>131</v>
+      </c>
+      <c r="C130">
+        <v>14701487</v>
+      </c>
+      <c r="D130">
+        <v>5.07</v>
+      </c>
+    </row>
+    <row r="131" spans="1:4">
+      <c r="A131" s="1">
+        <v>129</v>
+      </c>
+      <c r="B131" t="s">
+        <v>132</v>
+      </c>
+      <c r="C131">
+        <v>14829981</v>
+      </c>
+      <c r="D131">
+        <v>5.37</v>
+      </c>
+    </row>
+    <row r="132" spans="1:4">
+      <c r="A132" s="1">
+        <v>130</v>
+      </c>
+      <c r="B132" t="s">
+        <v>133</v>
+      </c>
+      <c r="C132">
+        <v>14965625</v>
+      </c>
+      <c r="D132">
+        <v>5.45</v>
+      </c>
+    </row>
+    <row r="133" spans="1:4">
+      <c r="A133" s="1">
+        <v>131</v>
+      </c>
+      <c r="B133" t="s">
+        <v>134</v>
+      </c>
+      <c r="C133">
+        <v>14738783</v>
+      </c>
+      <c r="D133">
+        <v>5.23</v>
+      </c>
+    </row>
+    <row r="134" spans="1:4">
+      <c r="A134" s="1">
+        <v>132</v>
+      </c>
+      <c r="B134" t="s">
+        <v>135</v>
+      </c>
+      <c r="C134">
+        <v>14787440</v>
+      </c>
+      <c r="D134">
+        <v>5.05</v>
+      </c>
+    </row>
+    <row r="135" spans="1:4">
+      <c r="A135" s="1">
+        <v>133</v>
+      </c>
+      <c r="B135" t="s">
+        <v>136</v>
+      </c>
+      <c r="C135">
+        <v>14893818</v>
+      </c>
+      <c r="D135">
+        <v>4.85</v>
+      </c>
+    </row>
+    <row r="136" spans="1:4">
+      <c r="A136" s="1">
+        <v>134</v>
+      </c>
+      <c r="B136" t="s">
+        <v>137</v>
+      </c>
+      <c r="C136">
+        <v>15003502</v>
+      </c>
+      <c r="D136">
+        <v>4.62</v>
+      </c>
+    </row>
+    <row r="137" spans="1:4">
+      <c r="A137" s="1">
+        <v>135</v>
+      </c>
+      <c r="B137" t="s">
+        <v>138</v>
+      </c>
+      <c r="C137">
+        <v>15022588</v>
+      </c>
+      <c r="D137">
+        <v>4.26</v>
+      </c>
+    </row>
+    <row r="138" spans="1:4">
+      <c r="A138" s="1">
+        <v>136</v>
+      </c>
+      <c r="B138" t="s">
+        <v>139</v>
+      </c>
+      <c r="C138">
+        <v>15050810</v>
+      </c>
+      <c r="D138">
+        <v>4.27</v>
+      </c>
+    </row>
+    <row r="139" spans="1:4">
+      <c r="A139" s="1">
+        <v>137</v>
+      </c>
+      <c r="B139" t="s">
+        <v>140</v>
+      </c>
+      <c r="C139">
+        <v>15090360</v>
+      </c>
+      <c r="D139">
+        <v>4.21</v>
+      </c>
+    </row>
+    <row r="140" spans="1:4">
+      <c r="A140" s="1">
+        <v>138</v>
+      </c>
+      <c r="B140" t="s">
+        <v>141</v>
+      </c>
+      <c r="C140">
+        <v>15131332</v>
+      </c>
+      <c r="D140">
+        <v>4.22</v>
+      </c>
+    </row>
+    <row r="141" spans="1:4">
+      <c r="A141" s="1">
+        <v>139</v>
+      </c>
+      <c r="B141" t="s">
+        <v>142</v>
+      </c>
+      <c r="C141">
+        <v>15202180</v>
+      </c>
+      <c r="D141">
+        <v>4.17</v>
+      </c>
+    </row>
+    <row r="142" spans="1:4">
+      <c r="A142" s="1">
+        <v>140</v>
+      </c>
+      <c r="B142" t="s">
+        <v>143</v>
+      </c>
+      <c r="C142">
+        <v>15315651</v>
+      </c>
+      <c r="D142">
+        <v>4.18</v>
+      </c>
+    </row>
+    <row r="143" spans="1:4">
+      <c r="A143" s="1">
+        <v>141</v>
+      </c>
+      <c r="B143" t="s">
+        <v>144</v>
+      </c>
+      <c r="C143">
+        <v>15445527</v>
+      </c>
+      <c r="D143">
+        <v>4.15</v>
+      </c>
+    </row>
+    <row r="144" spans="1:4">
+      <c r="A144" s="1">
+        <v>142</v>
+      </c>
+      <c r="B144" t="s">
+        <v>145</v>
+      </c>
+      <c r="C144">
+        <v>15550167</v>
+      </c>
+      <c r="D144">
+        <v>3.91</v>
+      </c>
+    </row>
+    <row r="145" spans="1:4">
+      <c r="A145" s="1">
+        <v>143</v>
+      </c>
+      <c r="B145" t="s">
+        <v>146</v>
+      </c>
+      <c r="C145">
+        <v>15350335</v>
+      </c>
+      <c r="D145">
+        <v>4.15</v>
+      </c>
+    </row>
+    <row r="146" spans="1:4">
+      <c r="A146" s="1">
+        <v>144</v>
+      </c>
+      <c r="B146" t="s">
+        <v>147</v>
+      </c>
+      <c r="C146">
+        <v>15427859</v>
+      </c>
+      <c r="D146">
+        <v>4.33</v>
+      </c>
+    </row>
+    <row r="147" spans="1:4">
+      <c r="A147" s="1">
+        <v>145</v>
+      </c>
+      <c r="B147" t="s">
+        <v>148</v>
+      </c>
+      <c r="C147">
+        <v>15563594</v>
+      </c>
+      <c r="D147">
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="148" spans="1:4">
+      <c r="A148" s="1">
+        <v>146</v>
+      </c>
+      <c r="B148" t="s">
+        <v>149</v>
+      </c>
+      <c r="C148">
+        <v>15695679</v>
+      </c>
+      <c r="D148">
+        <v>4.61</v>
+      </c>
+    </row>
+    <row r="149" spans="1:4">
+      <c r="A149" s="1">
+        <v>147</v>
+      </c>
+      <c r="B149" t="s">
+        <v>150</v>
+      </c>
+      <c r="C149">
+        <v>15706159</v>
+      </c>
+      <c r="D149">
+        <v>4.55</v>
+      </c>
+    </row>
+    <row r="150" spans="1:4">
+      <c r="A150" s="1">
+        <v>148</v>
+      </c>
+      <c r="B150" t="s">
+        <v>151</v>
+      </c>
+      <c r="C150">
+        <v>15731556</v>
+      </c>
+      <c r="D150">
+        <v>4.52</v>
+      </c>
+    </row>
+    <row r="151" spans="1:4">
+      <c r="A151" s="1">
+        <v>149</v>
+      </c>
+      <c r="B151" t="s">
+        <v>152</v>
+      </c>
+      <c r="C151">
+        <v>15806830</v>
+      </c>
+      <c r="D151">
+        <v>4.75</v>
+      </c>
+    </row>
+    <row r="152" spans="1:4">
+      <c r="A152" s="1">
+        <v>150</v>
+      </c>
+      <c r="B152" t="s">
+        <v>153</v>
+      </c>
+      <c r="C152">
+        <v>15849227</v>
+      </c>
+      <c r="D152">
+        <v>4.74</v>
+      </c>
+    </row>
+    <row r="153" spans="1:4">
+      <c r="A153" s="1">
+        <v>151</v>
+      </c>
+      <c r="B153" t="s">
+        <v>154</v>
+      </c>
+      <c r="C153">
+        <v>15920256</v>
+      </c>
+      <c r="D153">
+        <v>4.72</v>
+      </c>
+    </row>
+    <row r="154" spans="1:4">
+      <c r="A154" s="1">
+        <v>152</v>
+      </c>
+      <c r="B154" t="s">
+        <v>155</v>
+      </c>
+      <c r="C154">
+        <v>16033095</v>
+      </c>
+      <c r="D154">
+        <v>4.68</v>
+      </c>
+    </row>
+    <row r="155" spans="1:4">
+      <c r="A155" s="1">
+        <v>153</v>
+      </c>
+      <c r="B155" t="s">
+        <v>156</v>
+      </c>
+      <c r="C155">
+        <v>16182408</v>
+      </c>
+      <c r="D155">
+        <v>4.77</v>
+      </c>
+    </row>
+    <row r="156" spans="1:4">
+      <c r="A156" s="1">
+        <v>154</v>
+      </c>
+      <c r="B156" t="s">
+        <v>157</v>
+      </c>
+      <c r="C156">
+        <v>16294936</v>
+      </c>
+      <c r="D156">
+        <v>4.79</v>
+      </c>
+    </row>
+    <row r="157" spans="1:4">
+      <c r="A157" s="1">
+        <v>155</v>
+      </c>
+      <c r="B157" t="s">
+        <v>158</v>
+      </c>
+      <c r="C157">
+        <v>16062043</v>
+      </c>
+      <c r="D157">
+        <v>4.64</v>
+      </c>
+    </row>
+    <row r="158" spans="1:4">
+      <c r="A158" s="1">
+        <v>156</v>
+      </c>
+      <c r="B158" t="s">
+        <v>159</v>
+      </c>
+      <c r="C158">
+        <v>16106212</v>
+      </c>
+      <c r="D158">
+        <v>4.4</v>
+      </c>
+    </row>
+    <row r="159" spans="1:4">
+      <c r="A159" s="1">
+        <v>157</v>
+      </c>
+      <c r="B159" t="s">
+        <v>160</v>
+      </c>
+      <c r="C159">
+        <v>16227085</v>
+      </c>
+      <c r="D159">
+        <v>4.26</v>
+      </c>
+    </row>
+    <row r="160" spans="1:4">
+      <c r="A160" s="1">
+        <v>158</v>
+      </c>
+      <c r="B160" t="s">
+        <v>161</v>
+      </c>
+      <c r="C160">
+        <v>16281079</v>
+      </c>
+      <c r="D160">
+        <v>3.73</v>
+      </c>
+    </row>
+    <row r="161" spans="1:4">
+      <c r="A161" s="1">
+        <v>159</v>
+      </c>
+      <c r="B161" t="s">
+        <v>162</v>
+      </c>
+      <c r="C161">
+        <v>16347973</v>
+      </c>
+      <c r="D161">
+        <v>4.09</v>
+      </c>
+    </row>
+    <row r="162" spans="1:4">
+      <c r="A162" s="1">
+        <v>160</v>
+      </c>
+      <c r="B162" t="s">
+        <v>163</v>
+      </c>
+      <c r="C162">
+        <v>16354902</v>
+      </c>
+      <c r="D162">
+        <v>3.96</v>
+      </c>
+    </row>
+    <row r="163" spans="1:4">
+      <c r="A163" s="1">
+        <v>161</v>
+      </c>
+      <c r="B163" t="s">
+        <v>164</v>
+      </c>
+      <c r="C163">
+        <v>16357421</v>
+      </c>
+      <c r="D163">
+        <v>3.48</v>
+      </c>
+    </row>
+    <row r="164" spans="1:4">
+      <c r="A164" s="1">
+        <v>162</v>
+      </c>
+      <c r="B164" t="s">
+        <v>165</v>
+      </c>
+      <c r="C164">
+        <v>16362732</v>
+      </c>
+      <c r="D164">
+        <v>3.24</v>
+      </c>
+    </row>
+    <row r="165" spans="1:4">
+      <c r="A165" s="1">
+        <v>163</v>
+      </c>
+      <c r="B165" t="s">
+        <v>166</v>
+      </c>
+      <c r="C165">
+        <v>16414905</v>
+      </c>
+      <c r="D165">
+        <v>3.11</v>
+      </c>
+    </row>
+    <row r="166" spans="1:4">
+      <c r="A166" s="1">
+        <v>164</v>
+      </c>
+      <c r="B166" t="s">
+        <v>167</v>
+      </c>
+      <c r="C166">
+        <v>16508845</v>
+      </c>
+      <c r="D166">
+        <v>2.97</v>
+      </c>
+    </row>
+    <row r="167" spans="1:4">
+      <c r="A167" s="1">
+        <v>165</v>
+      </c>
+      <c r="B167" t="s">
+        <v>168</v>
+      </c>
+      <c r="C167">
+        <v>16652436</v>
+      </c>
+      <c r="D167">
+        <v>2.9</v>
+      </c>
+    </row>
+    <row r="168" spans="1:4">
+      <c r="A168" s="1">
+        <v>166</v>
+      </c>
+      <c r="B168" t="s">
+        <v>169</v>
+      </c>
+      <c r="C168">
+        <v>16772971</v>
+      </c>
+      <c r="D168">
+        <v>2.93</v>
+      </c>
+    </row>
+    <row r="169" spans="1:4">
+      <c r="A169" s="1">
+        <v>167</v>
+      </c>
+      <c r="B169" t="s">
+        <v>170</v>
+      </c>
+      <c r="C169">
+        <v>16525061</v>
+      </c>
+      <c r="D169">
+        <v>2.88</v>
+      </c>
+    </row>
+    <row r="170" spans="1:4">
+      <c r="A170" s="1">
+        <v>168</v>
+      </c>
+      <c r="B170" t="s">
+        <v>171</v>
+      </c>
+      <c r="C170">
+        <v>16547040</v>
+      </c>
+      <c r="D170">
+        <v>2.74</v>
+      </c>
+    </row>
+    <row r="171" spans="1:4">
+      <c r="A171" s="1">
+        <v>169</v>
+      </c>
+      <c r="B171" t="s">
+        <v>172</v>
+      </c>
+      <c r="C171">
+        <v>16672599</v>
+      </c>
+      <c r="D171">
+        <v>2.75</v>
+      </c>
+    </row>
+    <row r="172" spans="1:4">
+      <c r="A172" s="1">
+        <v>170</v>
+      </c>
+      <c r="B172" t="s">
+        <v>173</v>
+      </c>
+      <c r="C172">
+        <v>16781325</v>
+      </c>
+      <c r="D172">
+        <v>3.07</v>
+      </c>
+    </row>
+    <row r="173" spans="1:4">
+      <c r="A173" s="1">
+        <v>171</v>
+      </c>
+      <c r="B173" t="s">
+        <v>174</v>
+      </c>
+      <c r="C173">
+        <v>16837367</v>
+      </c>
+      <c r="D173">
+        <v>2.99</v>
+      </c>
+    </row>
+    <row r="174" spans="1:4">
+      <c r="A174" s="1">
+        <v>172</v>
+      </c>
+      <c r="B174" t="s">
+        <v>175</v>
+      </c>
+      <c r="C174">
+        <v>16885220</v>
+      </c>
+      <c r="D174">
+        <v>3.24</v>
+      </c>
+    </row>
+    <row r="175" spans="1:4">
+      <c r="A175" s="1">
+        <v>173</v>
+      </c>
+      <c r="B175" t="s">
+        <v>176</v>
+      </c>
+      <c r="C175">
+        <v>16928515</v>
+      </c>
+      <c r="D175">
+        <v>3.49</v>
+      </c>
+    </row>
+    <row r="176" spans="1:4">
+      <c r="A176" s="1">
+        <v>174</v>
+      </c>
+      <c r="B176" t="s">
+        <v>177</v>
+      </c>
+      <c r="C176">
+        <v>16965972</v>
+      </c>
+      <c r="D176">
+        <v>3.69</v>
+      </c>
+    </row>
+    <row r="177" spans="1:4">
+      <c r="A177" s="1">
+        <v>175</v>
+      </c>
+      <c r="B177" t="s">
+        <v>178</v>
+      </c>
+      <c r="C177">
+        <v>17023661</v>
+      </c>
+      <c r="D177">
+        <v>3.71</v>
+      </c>
+    </row>
+    <row r="178" spans="1:4">
+      <c r="A178" s="1">
+        <v>176</v>
+      </c>
+      <c r="B178" t="s">
+        <v>179</v>
+      </c>
+      <c r="C178">
+        <v>17180093</v>
+      </c>
+      <c r="D178">
+        <v>4.07</v>
+      </c>
+    </row>
+    <row r="179" spans="1:4">
+      <c r="A179" s="1">
+        <v>177</v>
+      </c>
+      <c r="B179" t="s">
+        <v>180</v>
+      </c>
+      <c r="C179">
+        <v>17352227</v>
+      </c>
+      <c r="D179">
+        <v>4.2</v>
+      </c>
+    </row>
+    <row r="180" spans="1:4">
+      <c r="A180" s="1">
+        <v>178</v>
+      </c>
+      <c r="B180" t="s">
+        <v>181</v>
+      </c>
+      <c r="C180">
+        <v>17475077</v>
+      </c>
+      <c r="D180">
+        <v>4.19</v>
+      </c>
+    </row>
+    <row r="181" spans="1:4">
+      <c r="A181" s="1">
+        <v>179</v>
+      </c>
+      <c r="B181" t="s">
+        <v>182</v>
+      </c>
+      <c r="C181">
+        <v>17239587</v>
+      </c>
+      <c r="D181">
+        <v>4.32</v>
+      </c>
+    </row>
+    <row r="182" spans="1:4">
+      <c r="A182" s="1">
+        <v>180</v>
+      </c>
+      <c r="B182" t="s">
+        <v>183</v>
+      </c>
+      <c r="C182">
+        <v>17299371</v>
+      </c>
+      <c r="D182">
+        <v>4.55</v>
+      </c>
+    </row>
+    <row r="183" spans="1:4">
+      <c r="A183" s="1">
+        <v>181</v>
+      </c>
+      <c r="B183" t="s">
+        <v>184</v>
+      </c>
+      <c r="C183">
+        <v>17433062</v>
+      </c>
+      <c r="D183">
+        <v>4.56</v>
+      </c>
+    </row>
+    <row r="184" spans="1:4">
+      <c r="A184" s="1">
+        <v>182</v>
+      </c>
+      <c r="B184" t="s">
+        <v>185</v>
+      </c>
+      <c r="C184">
+        <v>17538198</v>
+      </c>
+      <c r="D184">
+        <v>4.51</v>
+      </c>
+    </row>
+    <row r="185" spans="1:4">
+      <c r="A185" s="1">
+        <v>183</v>
+      </c>
+      <c r="B185" t="s">
+        <v>186</v>
+      </c>
+      <c r="C185">
+        <v>17603315</v>
+      </c>
+      <c r="D185">
+        <v>4.55</v>
+      </c>
+    </row>
+    <row r="186" spans="1:4">
+      <c r="A186" s="1">
+        <v>184</v>
+      </c>
+      <c r="B186" t="s">
+        <v>187</v>
+      </c>
+      <c r="C186">
+        <v>17595860</v>
+      </c>
+      <c r="D186">
+        <v>4.21</v>
+      </c>
+    </row>
+    <row r="187" spans="1:4">
+      <c r="A187" s="1">
+        <v>185</v>
+      </c>
+      <c r="B187" t="s">
+        <v>188</v>
+      </c>
+      <c r="C187">
+        <v>17674295</v>
+      </c>
+      <c r="D187">
+        <v>4.41</v>
+      </c>
+    </row>
+    <row r="188" spans="1:4">
+      <c r="A188" s="1">
+        <v>186</v>
+      </c>
+      <c r="B188" t="s">
+        <v>189</v>
+      </c>
+      <c r="C188">
+        <v>17718986</v>
+      </c>
+      <c r="D188">
+        <v>4.44</v>
+      </c>
+    </row>
+    <row r="189" spans="1:4">
+      <c r="A189" s="1">
+        <v>187</v>
+      </c>
+      <c r="B189" t="s">
+        <v>190</v>
+      </c>
+      <c r="C189">
+        <v>17791345</v>
+      </c>
+      <c r="D189">
+        <v>4.51</v>
+      </c>
+    </row>
+    <row r="190" spans="1:4">
+      <c r="A190" s="1">
+        <v>188</v>
+      </c>
+      <c r="B190" t="s">
+        <v>191</v>
+      </c>
+      <c r="C190">
+        <v>17908989</v>
+      </c>
+      <c r="D190">
+        <v>4.24</v>
+      </c>
+    </row>
+    <row r="191" spans="1:4">
+      <c r="A191" s="1">
+        <v>189</v>
+      </c>
+      <c r="B191" t="s">
+        <v>192</v>
+      </c>
+      <c r="C191">
+        <v>18055468</v>
+      </c>
+      <c r="D191">
+        <v>4.05</v>
+      </c>
+    </row>
+    <row r="192" spans="1:4">
+      <c r="A192" s="1">
+        <v>190</v>
+      </c>
+      <c r="B192" t="s">
+        <v>193</v>
+      </c>
+      <c r="C192">
+        <v>18187747</v>
+      </c>
+      <c r="D192">
+        <v>4.08</v>
+      </c>
+    </row>
+    <row r="193" spans="1:4">
+      <c r="A193" s="1">
+        <v>191</v>
+      </c>
+      <c r="B193" t="s">
+        <v>194</v>
+      </c>
+      <c r="C193">
+        <v>17884033</v>
+      </c>
+      <c r="D193">
+        <v>3.74</v>
+      </c>
+    </row>
+    <row r="194" spans="1:4">
+      <c r="A194" s="1">
+        <v>192</v>
+      </c>
+      <c r="B194" t="s">
+        <v>195</v>
+      </c>
+      <c r="C194">
+        <v>17953203</v>
+      </c>
+      <c r="D194">
+        <v>3.78</v>
+      </c>
+    </row>
+    <row r="195" spans="1:4">
+      <c r="A195" s="1">
+        <v>193</v>
+      </c>
+      <c r="B195" t="s">
+        <v>196</v>
+      </c>
+      <c r="C195">
+        <v>18095494</v>
+      </c>
+      <c r="D195">
+        <v>3.8</v>
+      </c>
+    </row>
+    <row r="196" spans="1:4">
+      <c r="A196" s="1">
+        <v>194</v>
+      </c>
+      <c r="B196" t="s">
+        <v>197</v>
+      </c>
+      <c r="C196">
+        <v>18154906</v>
+      </c>
+      <c r="D196">
+        <v>3.52</v>
+      </c>
+    </row>
+    <row r="197" spans="1:4">
+      <c r="A197" s="1">
+        <v>195</v>
+      </c>
+      <c r="B197" t="s">
+        <v>198</v>
+      </c>
+      <c r="C197">
+        <v>18237468</v>
+      </c>
+      <c r="D197">
+        <v>3.6</v>
+      </c>
+    </row>
+    <row r="198" spans="1:4">
+      <c r="A198" s="1">
+        <v>196</v>
+      </c>
+      <c r="B198" t="s">
+        <v>199</v>
+      </c>
+      <c r="C198">
+        <v>18257802</v>
+      </c>
+      <c r="D198">
+        <v>3.76</v>
+      </c>
+    </row>
+    <row r="199" spans="1:4">
+      <c r="A199" s="1">
+        <v>197</v>
+      </c>
+      <c r="B199" t="s">
+        <v>200</v>
+      </c>
+      <c r="C199">
+        <v>18326071</v>
+      </c>
+      <c r="D199">
+        <v>3.69</v>
+      </c>
+    </row>
+    <row r="200" spans="1:4">
+      <c r="A200" s="1">
+        <v>198</v>
+      </c>
+      <c r="B200" t="s">
+        <v>201</v>
+      </c>
+      <c r="C200">
+        <v>18348131</v>
+      </c>
+      <c r="D200">
+        <v>3.55</v>
+      </c>
+    </row>
+    <row r="201" spans="1:4">
+      <c r="A201" s="1">
+        <v>199</v>
+      </c>
+      <c r="B201" t="s">
+        <v>202</v>
+      </c>
+      <c r="C201">
+        <v>18466227</v>
+      </c>
+      <c r="D201">
+        <v>3.79</v>
+      </c>
+    </row>
+    <row r="202" spans="1:4">
+      <c r="A202" s="1">
+        <v>200</v>
+      </c>
+      <c r="B202" t="s">
+        <v>203</v>
+      </c>
+      <c r="C202">
+        <v>18626402</v>
+      </c>
+      <c r="D202">
+        <v>4.01</v>
+      </c>
+    </row>
+    <row r="203" spans="1:4">
+      <c r="A203" s="1">
+        <v>201</v>
+      </c>
+      <c r="B203" t="s">
+        <v>204</v>
+      </c>
+      <c r="C203">
+        <v>18797954</v>
+      </c>
+      <c r="D203">
+        <v>4.11</v>
+      </c>
+    </row>
+    <row r="204" spans="1:4">
+      <c r="A204" s="1">
+        <v>202</v>
+      </c>
+      <c r="B204" t="s">
+        <v>205</v>
+      </c>
+      <c r="C204">
+        <v>18935841</v>
+      </c>
+      <c r="D204">
+        <v>4.11</v>
+      </c>
+    </row>
+    <row r="205" spans="1:4">
+      <c r="A205" s="1">
+        <v>203</v>
+      </c>
+      <c r="B205" t="s">
+        <v>206</v>
+      </c>
+      <c r="C205">
+        <v>18616624</v>
+      </c>
+      <c r="D205">
+        <v>4.1</v>
+      </c>
+    </row>
+    <row r="206" spans="1:4">
+      <c r="A206" s="1">
+        <v>204</v>
+      </c>
+      <c r="B206" t="s">
+        <v>207</v>
+      </c>
+      <c r="C206">
+        <v>18699916</v>
+      </c>
+      <c r="D206">
+        <v>4.16</v>
+      </c>
+    </row>
+    <row r="207" spans="1:4">
+      <c r="A207" s="1">
+        <v>205</v>
+      </c>
+      <c r="B207" t="s">
+        <v>208</v>
+      </c>
+      <c r="C207">
+        <v>18853971</v>
+      </c>
+      <c r="D207">
+        <v>4.19</v>
+      </c>
+    </row>
+    <row r="208" spans="1:4">
+      <c r="A208" s="1">
+        <v>206</v>
+      </c>
+      <c r="B208" t="s">
+        <v>209</v>
+      </c>
+      <c r="C208">
+        <v>18994318</v>
+      </c>
+      <c r="D208">
+        <v>4.62</v>
+      </c>
+    </row>
+    <row r="209" spans="1:4">
+      <c r="A209" s="1">
+        <v>207</v>
+      </c>
+      <c r="B209" t="s">
+        <v>210</v>
+      </c>
+      <c r="C209">
+        <v>19021083</v>
+      </c>
+      <c r="D209">
+        <v>4.3</v>
+      </c>
+    </row>
+    <row r="210" spans="1:4">
+      <c r="A210" s="1">
+        <v>208</v>
+      </c>
+      <c r="B210" t="s">
+        <v>211</v>
+      </c>
+      <c r="C210">
+        <v>19047825</v>
+      </c>
+      <c r="D210">
+        <v>4.33</v>
+      </c>
+    </row>
+    <row r="211" spans="1:4">
+      <c r="A211" s="1">
+        <v>209</v>
+      </c>
+      <c r="B211" t="s">
+        <v>212</v>
+      </c>
+      <c r="C211">
+        <v>19134058</v>
+      </c>
+      <c r="D211">
+        <v>4.41</v>
+      </c>
+    </row>
+    <row r="212" spans="1:4">
+      <c r="A212" s="1">
+        <v>210</v>
+      </c>
+      <c r="B212" t="s">
+        <v>213</v>
+      </c>
+      <c r="C212">
+        <v>19172222</v>
+      </c>
+      <c r="D212">
+        <v>4.49</v>
+      </c>
+    </row>
+    <row r="213" spans="1:4">
+      <c r="A213" s="1">
+        <v>211</v>
+      </c>
+      <c r="B213" t="s">
+        <v>214</v>
+      </c>
+      <c r="C213">
+        <v>19292865</v>
+      </c>
+      <c r="D213">
+        <v>4.48</v>
+      </c>
+    </row>
+    <row r="214" spans="1:4">
+      <c r="A214" s="1">
+        <v>212</v>
+      </c>
+      <c r="B214" t="s">
+        <v>215</v>
+      </c>
+      <c r="C214">
+        <v>19428916</v>
+      </c>
+      <c r="D214">
+        <v>4.31</v>
+      </c>
+    </row>
+    <row r="215" spans="1:4">
+      <c r="A215" s="1">
+        <v>213</v>
+      </c>
+      <c r="B215" t="s">
+        <v>216</v>
+      </c>
+      <c r="C215">
+        <v>19623674</v>
+      </c>
+      <c r="D215">
+        <v>4.39</v>
+      </c>
+    </row>
+    <row r="216" spans="1:4">
+      <c r="A216" s="1">
+        <v>214</v>
+      </c>
+      <c r="B216" t="s">
+        <v>217</v>
+      </c>
+      <c r="C216">
+        <v>19755991</v>
+      </c>
+      <c r="D216">
+        <v>4.33</v>
+      </c>
+    </row>
+    <row r="217" spans="1:4">
+      <c r="A217" s="1">
+        <v>215</v>
+      </c>
+      <c r="B217" t="s">
+        <v>218</v>
+      </c>
+      <c r="C217">
+        <v>19418455</v>
+      </c>
+      <c r="D217">
+        <v>4.31</v>
+      </c>
+    </row>
+    <row r="218" spans="1:4">
+      <c r="A218" s="1">
+        <v>216</v>
+      </c>
+      <c r="B218" t="s">
+        <v>219</v>
+      </c>
+      <c r="C218">
+        <v>19532177</v>
+      </c>
+      <c r="D218">
+        <v>4.45</v>
+      </c>
+    </row>
+    <row r="219" spans="1:4">
+      <c r="A219" s="1">
+        <v>217</v>
+      </c>
+      <c r="B219" t="s">
+        <v>220</v>
+      </c>
+      <c r="C219">
+        <v>19696488</v>
+      </c>
+      <c r="D219">
+        <v>4.47</v>
+      </c>
+    </row>
+    <row r="220" spans="1:4">
+      <c r="A220" s="1">
+        <v>218</v>
+      </c>
+      <c r="B220" t="s">
+        <v>221</v>
+      </c>
+      <c r="C220">
+        <v>19786997</v>
+      </c>
+      <c r="D220">
+        <v>4.17</v>
+      </c>
+    </row>
+    <row r="221" spans="1:4">
+      <c r="A221" s="1">
+        <v>219</v>
+      </c>
+      <c r="B221" t="s">
+        <v>222</v>
+      </c>
+      <c r="C221">
+        <v>19874106</v>
+      </c>
+      <c r="D221">
+        <v>4.48</v>
+      </c>
+    </row>
+    <row r="222" spans="1:4">
+      <c r="A222" s="1">
+        <v>220</v>
+      </c>
+      <c r="B222" t="s">
+        <v>223</v>
+      </c>
+      <c r="C222">
+        <v>19908072</v>
+      </c>
+      <c r="D222">
+        <v>4.52</v>
+      </c>
+    </row>
+    <row r="223" spans="1:4">
+      <c r="A223" s="1">
+        <v>221</v>
+      </c>
+      <c r="B223" t="s">
+        <v>224</v>
+      </c>
+      <c r="C223">
+        <v>19894575</v>
+      </c>
+      <c r="D223">
+        <v>3.97</v>
+      </c>
+    </row>
+    <row r="224" spans="1:4">
+      <c r="A224" s="1">
+        <v>222</v>
+      </c>
+      <c r="B224" t="s">
+        <v>225</v>
+      </c>
+      <c r="C224">
+        <v>19949244</v>
+      </c>
+      <c r="D224">
+        <v>4.05</v>
+      </c>
+    </row>
+    <row r="225" spans="1:4">
+      <c r="A225" s="1">
+        <v>223</v>
+      </c>
+      <c r="B225" t="s">
+        <v>226</v>
+      </c>
+      <c r="C225">
+        <v>20063433</v>
+      </c>
+      <c r="D225">
+        <v>3.99</v>
+      </c>
+    </row>
+    <row r="226" spans="1:4">
+      <c r="A226" s="1">
+        <v>224</v>
+      </c>
+      <c r="B226" t="s">
+        <v>227</v>
+      </c>
+      <c r="C226">
+        <v>20192960</v>
+      </c>
+      <c r="D226">
+        <v>3.93</v>
+      </c>
+    </row>
+    <row r="227" spans="1:4">
+      <c r="A227" s="1">
+        <v>225</v>
+      </c>
+      <c r="B227" t="s">
+        <v>228</v>
+      </c>
+      <c r="C227">
+        <v>20356179</v>
+      </c>
+      <c r="D227">
+        <v>3.73</v>
+      </c>
+    </row>
+    <row r="228" spans="1:4">
+      <c r="A228" s="1">
+        <v>226</v>
+      </c>
+      <c r="B228" t="s">
+        <v>229</v>
+      </c>
+      <c r="C228">
+        <v>20457926</v>
+      </c>
+      <c r="D228">
+        <v>3.55</v>
+      </c>
+    </row>
+    <row r="229" spans="1:4">
+      <c r="A229" s="1">
+        <v>227</v>
+      </c>
+      <c r="B229" t="s">
+        <v>230</v>
+      </c>
+      <c r="C229">
+        <v>20079365</v>
+      </c>
+      <c r="D229">
+        <v>3.4</v>
+      </c>
+    </row>
+    <row r="230" spans="1:4">
+      <c r="A230" s="1">
+        <v>228</v>
+      </c>
+      <c r="B230" t="s">
+        <v>231</v>
+      </c>
+      <c r="C230">
+        <v>20174011</v>
+      </c>
+      <c r="D230">
+        <v>3.29</v>
+      </c>
+    </row>
+    <row r="231" spans="1:4">
+      <c r="A231" s="1">
+        <v>229</v>
+      </c>
+      <c r="B231" t="s">
+        <v>232</v>
+      </c>
+      <c r="C231">
+        <v>20299993</v>
+      </c>
+      <c r="D231">
+        <v>3.06</v>
+      </c>
+    </row>
+    <row r="232" spans="1:4">
+      <c r="A232" s="1">
+        <v>230</v>
+      </c>
+      <c r="B232" t="s">
+        <v>233</v>
+      </c>
+      <c r="C232">
+        <v>20348508</v>
+      </c>
+      <c r="D232">
+        <v>2.84</v>
+      </c>
+    </row>
+    <row r="233" spans="1:4">
+      <c r="A233" s="1">
+        <v>231</v>
+      </c>
+      <c r="B233" t="s">
+        <v>234</v>
+      </c>
+      <c r="C233">
+        <v>20378927</v>
+      </c>
+      <c r="D233">
+        <v>2.54</v>
+      </c>
+    </row>
+    <row r="234" spans="1:4">
+      <c r="A234" s="1">
+        <v>232</v>
+      </c>
+      <c r="B234" t="s">
+        <v>235</v>
+      </c>
+      <c r="C234">
+        <v>20382910</v>
+      </c>
+      <c r="D234">
+        <v>2.39</v>
+      </c>
+    </row>
+    <row r="235" spans="1:4">
+      <c r="A235" s="1">
+        <v>233</v>
+      </c>
+      <c r="B235" t="s">
+        <v>236</v>
+      </c>
+      <c r="C235">
+        <v>20368666</v>
+      </c>
+      <c r="D235">
+        <v>2.38</v>
+      </c>
+    </row>
+    <row r="236" spans="1:4">
+      <c r="A236" s="1">
+        <v>234</v>
+      </c>
+      <c r="B236" t="s">
+        <v>237</v>
+      </c>
+      <c r="C236">
+        <v>20385379</v>
+      </c>
+      <c r="D236">
+        <v>2.19</v>
+      </c>
+    </row>
+    <row r="237" spans="1:4">
+      <c r="A237" s="1">
+        <v>235</v>
+      </c>
+      <c r="B237" t="s">
+        <v>238</v>
+      </c>
+      <c r="C237">
+        <v>20422010</v>
+      </c>
+      <c r="D237">
+        <v>1.79</v>
+      </c>
+    </row>
+    <row r="238" spans="1:4">
+      <c r="A238" s="1">
+        <v>236</v>
+      </c>
+      <c r="B238" t="s">
+        <v>239</v>
+      </c>
+      <c r="C238">
+        <v>20567426</v>
+      </c>
+      <c r="D238">
+        <v>1.85</v>
+      </c>
+    </row>
+    <row r="239" spans="1:4">
+      <c r="A239" s="1">
+        <v>237</v>
+      </c>
+      <c r="B239" t="s">
+        <v>240</v>
+      </c>
+      <c r="C239">
+        <v>20727424</v>
+      </c>
+      <c r="D239">
+        <v>1.82</v>
+      </c>
+    </row>
+    <row r="240" spans="1:4">
+      <c r="A240" s="1">
+        <v>238</v>
+      </c>
+      <c r="B240" t="s">
+        <v>241</v>
+      </c>
+      <c r="C240">
+        <v>20803652</v>
+      </c>
+      <c r="D240">
+        <v>1.69</v>
+      </c>
+    </row>
+    <row r="241" spans="1:4">
+      <c r="A241" s="1">
+        <v>239</v>
+      </c>
+      <c r="B241" t="s">
+        <v>242</v>
+      </c>
+      <c r="C241">
+        <v>20421442</v>
+      </c>
+      <c r="D241">
+        <v>1.7</v>
+      </c>
+    </row>
+    <row r="242" spans="1:4">
+      <c r="A242" s="1">
+        <v>240</v>
+      </c>
+      <c r="B242" t="s">
+        <v>243</v>
+      </c>
+      <c r="C242">
+        <v>20490397</v>
+      </c>
+      <c r="D242">
+        <v>1.57</v>
+      </c>
+    </row>
+    <row r="243" spans="1:4">
+      <c r="A243" s="1">
+        <v>241</v>
+      </c>
+      <c r="B243" t="s">
+        <v>244</v>
+      </c>
+      <c r="C243">
+        <v>20613536</v>
+      </c>
+      <c r="D243">
+        <v>1.54</v>
+      </c>
+    </row>
+    <row r="244" spans="1:4">
+      <c r="A244" s="1">
+        <v>242</v>
+      </c>
+      <c r="B244" t="s">
+        <v>245</v>
+      </c>
+      <c r="C244">
+        <v>20482943</v>
+      </c>
+      <c r="D244">
+        <v>0.66</v>
+      </c>
+    </row>
+    <row r="245" spans="1:4">
+      <c r="A245" s="1">
+        <v>243</v>
+      </c>
+      <c r="B245" t="s">
+        <v>246</v>
+      </c>
+      <c r="C245">
+        <v>19927696</v>
+      </c>
+      <c r="D245">
+        <v>-2.21</v>
+      </c>
+    </row>
+    <row r="246" spans="1:4">
+      <c r="A246" s="1">
+        <v>244</v>
+      </c>
+      <c r="B246" t="s">
+        <v>247</v>
+      </c>
+      <c r="C246">
+        <v>19583170</v>
+      </c>
+      <c r="D246">
+        <v>-3.92</v>
+      </c>
+    </row>
+    <row r="247" spans="1:4">
+      <c r="A247" s="1">
+        <v>245</v>
+      </c>
+      <c r="B247" t="s">
+        <v>248</v>
+      </c>
+      <c r="C247">
+        <v>19499859</v>
+      </c>
+      <c r="D247">
+        <v>-4.27</v>
+      </c>
+    </row>
+    <row r="248" spans="1:4">
+      <c r="A248" s="1">
+        <v>246</v>
+      </c>
+      <c r="B248" t="s">
+        <v>249</v>
+      </c>
+      <c r="C248">
+        <v>19495952</v>
+      </c>
+      <c r="D248">
+        <v>-4.36</v>
+      </c>
+    </row>
+    <row r="249" spans="1:4">
+      <c r="A249" s="1">
+        <v>247</v>
+      </c>
+      <c r="B249" t="s">
+        <v>250</v>
+      </c>
+      <c r="C249">
+        <v>19588342</v>
+      </c>
+      <c r="D249">
+        <v>-4.08</v>
+      </c>
+    </row>
+    <row r="250" spans="1:4">
+      <c r="A250" s="1">
+        <v>248</v>
+      </c>
+      <c r="B250" t="s">
+        <v>251</v>
+      </c>
+      <c r="C250">
+        <v>19702192</v>
+      </c>
+      <c r="D250">
+        <v>-4.21</v>
+      </c>
+    </row>
+    <row r="251" spans="1:4">
+      <c r="A251" s="1">
+        <v>249</v>
+      </c>
+      <c r="B251" t="s">
+        <v>252</v>
+      </c>
+      <c r="C251">
+        <v>19902833</v>
+      </c>
+      <c r="D251">
+        <v>-3.98</v>
+      </c>
+    </row>
+    <row r="252" spans="1:4">
+      <c r="A252" s="1">
+        <v>250</v>
+      </c>
+      <c r="B252" t="s">
+        <v>253</v>
+      </c>
+      <c r="C252">
+        <v>20051552</v>
+      </c>
+      <c r="D252">
+        <v>-3.62</v>
+      </c>
+    </row>
+    <row r="253" spans="1:4">
+      <c r="A253" s="1">
+        <v>251</v>
+      </c>
+      <c r="B253" t="s">
+        <v>254</v>
+      </c>
+      <c r="C253">
+        <v>19773732</v>
+      </c>
+      <c r="D253">
+        <v>-3.17</v>
+      </c>
+    </row>
+    <row r="254" spans="1:4">
+      <c r="A254" s="1">
+        <v>252</v>
+      </c>
+      <c r="B254" t="s">
+        <v>255</v>
+      </c>
+      <c r="C254">
+        <v>19821651</v>
+      </c>
+      <c r="D254">
+        <v>-3.26</v>
+      </c>
+    </row>
+    <row r="255" spans="1:4">
+      <c r="A255" s="1">
+        <v>253</v>
+      </c>
+      <c r="B255" t="s">
+        <v>256</v>
+      </c>
+      <c r="C255">
+        <v>19936938</v>
+      </c>
+      <c r="D255">
+        <v>-3.28</v>
+      </c>
+    </row>
+    <row r="256" spans="1:4">
+      <c r="A256" s="1">
+        <v>254</v>
+      </c>
+      <c r="B256" t="s">
+        <v>257</v>
+      </c>
+      <c r="C256">
+        <v>20025709</v>
+      </c>
+      <c r="D256">
+        <v>-2.23</v>
+      </c>
+    </row>
+    <row r="257" spans="1:4">
+      <c r="A257" s="1">
+        <v>255</v>
+      </c>
+      <c r="B257" t="s">
+        <v>258</v>
+      </c>
+      <c r="C257">
+        <v>20070483</v>
+      </c>
+      <c r="D257">
+        <v>0.72</v>
+      </c>
+    </row>
+    <row r="258" spans="1:4">
+      <c r="A258" s="1">
+        <v>256</v>
+      </c>
+      <c r="B258" t="s">
+        <v>259</v>
+      </c>
+      <c r="C258">
+        <v>20109444</v>
+      </c>
+      <c r="D258">
+        <v>2.69</v>
+      </c>
+    </row>
+    <row r="259" spans="1:4">
+      <c r="A259" s="1">
+        <v>257</v>
+      </c>
+      <c r="B259" t="s">
+        <v>260</v>
+      </c>
+      <c r="C259">
+        <v>20175380</v>
+      </c>
+      <c r="D259">
+        <v>3.46</v>
+      </c>
+    </row>
+    <row r="260" spans="1:4">
+      <c r="A260" s="1">
+        <v>258</v>
+      </c>
+      <c r="B260" t="s">
+        <v>261</v>
+      </c>
+      <c r="C260">
+        <v>20291923</v>
+      </c>
+      <c r="D260">
+        <v>4.08</v>
+      </c>
+    </row>
+    <row r="261" spans="1:4">
+      <c r="A261" s="1">
+        <v>259</v>
+      </c>
+      <c r="B261" t="s">
+        <v>262</v>
+      </c>
+      <c r="C261">
+        <v>20420823</v>
+      </c>
+      <c r="D261">
+        <v>4.25</v>
+      </c>
+    </row>
+    <row r="262" spans="1:4">
+      <c r="A262" s="1">
+        <v>260</v>
+      </c>
+      <c r="B262" t="s">
+        <v>263</v>
+      </c>
+      <c r="C262">
+        <v>20594919</v>
+      </c>
+      <c r="D262">
+        <v>4.53</v>
+      </c>
+    </row>
+    <row r="263" spans="1:4">
+      <c r="A263" s="1">
+        <v>261</v>
+      </c>
+      <c r="B263" t="s">
+        <v>264</v>
+      </c>
+      <c r="C263">
+        <v>20767587</v>
+      </c>
+      <c r="D263">
+        <v>4.34</v>
+      </c>
+    </row>
+    <row r="264" spans="1:4">
+      <c r="A264" s="1">
+        <v>262</v>
+      </c>
+      <c r="B264" t="s">
+        <v>265</v>
+      </c>
+      <c r="C264">
+        <v>20933050</v>
+      </c>
+      <c r="D264">
+        <v>4.4</v>
+      </c>
+    </row>
+    <row r="265" spans="1:4">
+      <c r="A265" s="1">
+        <v>263</v>
+      </c>
+      <c r="B265" t="s">
+        <v>266</v>
+      </c>
+      <c r="C265">
+        <v>20620148</v>
+      </c>
+      <c r="D265">
+        <v>4.28</v>
+      </c>
+    </row>
+    <row r="266" spans="1:4">
+      <c r="A266" s="1">
+        <v>264</v>
+      </c>
+      <c r="B266" t="s">
+        <v>267</v>
+      </c>
+      <c r="C266">
+        <v>20762419</v>
+      </c>
+      <c r="D266">
+        <v>4.75</v>
+      </c>
+    </row>
+    <row r="267" spans="1:4">
+      <c r="A267" s="1">
+        <v>265</v>
+      </c>
+      <c r="B267" t="s">
+        <v>268</v>
+      </c>
+      <c r="C267">
+        <v>20941286</v>
+      </c>
+      <c r="D267">
+        <v>5.04</v>
+      </c>
+    </row>
+    <row r="268" spans="1:4">
+      <c r="A268" s="1">
+        <v>266</v>
+      </c>
+      <c r="B268" t="s">
+        <v>269</v>
+      </c>
+      <c r="C268">
+        <v>21005852</v>
+      </c>
+      <c r="D268">
+        <v>4.89</v>
+      </c>
+    </row>
+    <row r="269" spans="1:4">
+      <c r="A269" s="1">
+        <v>267</v>
+      </c>
+      <c r="B269" t="s">
+        <v>270</v>
+      </c>
+      <c r="C269">
+        <v>21011342</v>
+      </c>
+      <c r="D269">
+        <v>4.69</v>
+      </c>
+    </row>
+    <row r="270" spans="1:4">
+      <c r="A270" s="1">
+        <v>268</v>
+      </c>
+      <c r="B270" t="s">
+        <v>271</v>
+      </c>
+      <c r="C270">
+        <v>21008487</v>
+      </c>
+      <c r="D270">
+        <v>4.47</v>
+      </c>
+    </row>
+    <row r="271" spans="1:4">
+      <c r="A271" s="1">
+        <v>269</v>
+      </c>
+      <c r="B271" t="s">
+        <v>272</v>
+      </c>
+      <c r="C271">
+        <v>21068708</v>
+      </c>
+      <c r="D271">
+        <v>4.43</v>
+      </c>
+    </row>
+    <row r="272" spans="1:4">
+      <c r="A272" s="1">
+        <v>270</v>
+      </c>
+      <c r="B272" t="s">
+        <v>273</v>
+      </c>
+      <c r="C272">
+        <v>21079434</v>
+      </c>
+      <c r="D272">
+        <v>3.88</v>
+      </c>
+    </row>
+    <row r="273" spans="1:4">
+      <c r="A273" s="1">
+        <v>271</v>
+      </c>
+      <c r="B273" t="s">
+        <v>274</v>
+      </c>
+      <c r="C273">
+        <v>21236866</v>
+      </c>
+      <c r="D273">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="274" spans="1:4">
+      <c r="A274" s="1">
+        <v>272</v>
+      </c>
+      <c r="B274" t="s">
+        <v>275</v>
+      </c>
+      <c r="C274">
+        <v>21409358</v>
+      </c>
+      <c r="D274">
+        <v>3.95</v>
+      </c>
+    </row>
+    <row r="275" spans="1:4">
+      <c r="A275" s="1">
+        <v>273</v>
+      </c>
+      <c r="B275" t="s">
+        <v>276</v>
+      </c>
+      <c r="C275">
+        <v>21617326</v>
+      </c>
+      <c r="D275">
+        <v>4.09</v>
+      </c>
+    </row>
+    <row r="276" spans="1:4">
+      <c r="A276" s="1">
+        <v>274</v>
+      </c>
+      <c r="B276" t="s">
+        <v>277</v>
+      </c>
+      <c r="C276">
+        <v>21718601</v>
+      </c>
+      <c r="D276">
+        <v>3.75</v>
+      </c>
+    </row>
+    <row r="277" spans="1:4">
+      <c r="A277" s="1">
+        <v>275</v>
+      </c>
+      <c r="B277" t="s">
+        <v>278</v>
+      </c>
+      <c r="C277">
+        <v>21372896</v>
+      </c>
+      <c r="D277">
+        <v>3.65</v>
+      </c>
+    </row>
+    <row r="278" spans="1:4">
+      <c r="A278" s="1">
+        <v>276</v>
+      </c>
+      <c r="B278" t="s">
+        <v>279</v>
+      </c>
+      <c r="C278">
+        <v>21484595</v>
+      </c>
+      <c r="D278">
+        <v>3.48</v>
+      </c>
+    </row>
+    <row r="279" spans="1:4">
+      <c r="A279" s="1">
+        <v>277</v>
+      </c>
+      <c r="B279" t="s">
+        <v>280</v>
+      </c>
+      <c r="C279">
+        <v>21660469</v>
+      </c>
+      <c r="D279">
+        <v>3.43</v>
+      </c>
+    </row>
+    <row r="280" spans="1:4">
+      <c r="A280" s="1">
+        <v>278</v>
+      </c>
+      <c r="B280" t="s">
+        <v>281</v>
+      </c>
+      <c r="C280">
+        <v>21796280</v>
+      </c>
+      <c r="D280">
+        <v>3.76</v>
+      </c>
+    </row>
+    <row r="281" spans="1:4">
+      <c r="A281" s="1">
+        <v>279</v>
+      </c>
+      <c r="B281" t="s">
+        <v>282</v>
+      </c>
+      <c r="C281">
+        <v>21820291</v>
+      </c>
+      <c r="D281">
+        <v>3.85</v>
+      </c>
+    </row>
+    <row r="282" spans="1:4">
+      <c r="A282" s="1">
+        <v>280</v>
+      </c>
+      <c r="B282" t="s">
+        <v>283</v>
+      </c>
+      <c r="C282">
+        <v>21862909</v>
+      </c>
+      <c r="D282">
+        <v>4.07</v>
+      </c>
+    </row>
+    <row r="283" spans="1:4">
+      <c r="A283" s="1">
+        <v>281</v>
+      </c>
+      <c r="B283" t="s">
+        <v>284</v>
+      </c>
+      <c r="C283">
+        <v>21887307</v>
+      </c>
+      <c r="D283">
+        <v>3.89</v>
+      </c>
+    </row>
+    <row r="284" spans="1:4">
+      <c r="A284" s="1">
+        <v>282</v>
+      </c>
+      <c r="B284" t="s">
+        <v>285</v>
+      </c>
+      <c r="C284">
+        <v>21885139</v>
+      </c>
+      <c r="D284">
+        <v>3.82</v>
+      </c>
+    </row>
+    <row r="285" spans="1:4">
+      <c r="A285" s="1">
+        <v>283</v>
+      </c>
+      <c r="B285" t="s">
+        <v>286</v>
+      </c>
+      <c r="C285">
+        <v>21996875</v>
+      </c>
+      <c r="D285">
+        <v>3.58</v>
+      </c>
+    </row>
+    <row r="286" spans="1:4">
+      <c r="A286" s="1">
+        <v>284</v>
+      </c>
+      <c r="B286" t="s">
+        <v>287</v>
+      </c>
+      <c r="C286">
+        <v>22129433</v>
+      </c>
+      <c r="D286">
+        <v>3.36</v>
+      </c>
+    </row>
+    <row r="287" spans="1:4">
+      <c r="A287" s="1">
+        <v>285</v>
+      </c>
+      <c r="B287" t="s">
+        <v>288</v>
+      </c>
+      <c r="C287">
+        <v>22302690</v>
+      </c>
+      <c r="D287">
+        <v>3.17</v>
+      </c>
+    </row>
+    <row r="288" spans="1:4">
+      <c r="A288" s="1">
+        <v>286</v>
+      </c>
+      <c r="B288" t="s">
+        <v>289</v>
+      </c>
+      <c r="C288">
+        <v>22409268</v>
+      </c>
+      <c r="D288">
+        <v>3.18</v>
+      </c>
+    </row>
+    <row r="289" spans="1:4">
+      <c r="A289" s="1">
+        <v>287</v>
+      </c>
+      <c r="B289" t="s">
+        <v>290</v>
+      </c>
+      <c r="C289">
+        <v>22024386</v>
+      </c>
+      <c r="D289">
+        <v>3.05</v>
+      </c>
+    </row>
+    <row r="290" spans="1:4">
+      <c r="A290" s="1">
+        <v>288</v>
+      </c>
+      <c r="B290" t="s">
+        <v>291</v>
+      </c>
+      <c r="C290">
+        <v>22133407</v>
+      </c>
+      <c r="D290">
+        <v>3.02</v>
+      </c>
+    </row>
+    <row r="291" spans="1:4">
+      <c r="A291" s="1">
+        <v>289</v>
+      </c>
+      <c r="B291" t="s">
+        <v>292</v>
+      </c>
+      <c r="C291">
+        <v>22289810</v>
+      </c>
+      <c r="D291">
+        <v>2.91</v>
+      </c>
+    </row>
+    <row r="292" spans="1:4">
+      <c r="A292" s="1">
+        <v>290</v>
+      </c>
+      <c r="B292" t="s">
+        <v>293</v>
+      </c>
+      <c r="C292">
+        <v>22289345</v>
+      </c>
+      <c r="D292">
+        <v>2.26</v>
+      </c>
+    </row>
+    <row r="293" spans="1:4">
+      <c r="A293" s="1">
+        <v>291</v>
+      </c>
+      <c r="B293" t="s">
+        <v>294</v>
+      </c>
+      <c r="C293">
+        <v>22374202</v>
+      </c>
+      <c r="D293">
+        <v>2.54</v>
+      </c>
+    </row>
+    <row r="294" spans="1:4">
+      <c r="A294" s="1">
+        <v>292</v>
+      </c>
+      <c r="B294" t="s">
+        <v>295</v>
+      </c>
+      <c r="C294">
+        <v>22348999</v>
+      </c>
+      <c r="D294">
+        <v>2.22</v>
+      </c>
+    </row>
+    <row r="295" spans="1:4">
+      <c r="A295" s="1">
+        <v>293</v>
+      </c>
+      <c r="B295" t="s">
+        <v>296</v>
+      </c>
+      <c r="C295">
+        <v>22319444</v>
+      </c>
+      <c r="D295">
+        <v>1.97</v>
+      </c>
+    </row>
+    <row r="296" spans="1:4">
+      <c r="A296" s="1">
+        <v>294</v>
+      </c>
+      <c r="B296" t="s">
+        <v>297</v>
+      </c>
+      <c r="C296">
+        <v>22331788</v>
+      </c>
+      <c r="D296">
+        <v>2.04</v>
+      </c>
+    </row>
+    <row r="297" spans="1:4">
+      <c r="A297" s="1">
+        <v>295</v>
+      </c>
+      <c r="B297" t="s">
+        <v>298</v>
+      </c>
+      <c r="C297">
+        <v>22389835</v>
+      </c>
+      <c r="D297">
+        <v>1.79</v>
+      </c>
+    </row>
+    <row r="298" spans="1:4">
+      <c r="A298" s="1">
+        <v>296</v>
+      </c>
+      <c r="B298" t="s">
+        <v>299</v>
+      </c>
+      <c r="C298">
+        <v>22480803</v>
+      </c>
+      <c r="D298">
+        <v>1.59</v>
+      </c>
+    </row>
+    <row r="299" spans="1:4">
+      <c r="A299" s="1">
+        <v>297</v>
+      </c>
+      <c r="B299" t="s">
+        <v>300</v>
+      </c>
+      <c r="C299">
+        <v>22618942</v>
+      </c>
+      <c r="D299">
+        <v>1.42</v>
+      </c>
+    </row>
+    <row r="300" spans="1:4">
+      <c r="A300" s="1">
+        <v>298</v>
+      </c>
+      <c r="B300" t="s">
+        <v>301</v>
+      </c>
+      <c r="C300">
+        <v>22643638</v>
+      </c>
+      <c r="D300">
+        <v>1.05</v>
+      </c>
+    </row>
+    <row r="301" spans="1:4">
+      <c r="A301" s="1">
+        <v>299</v>
+      </c>
+      <c r="B301" t="s">
+        <v>302</v>
+      </c>
+      <c r="C301">
+        <v>22238379</v>
+      </c>
+      <c r="D301">
+        <v>0.97</v>
+      </c>
+    </row>
+    <row r="302" spans="1:4">
+      <c r="A302" s="1">
+        <v>300</v>
+      </c>
+      <c r="B302" t="s">
+        <v>303</v>
+      </c>
+      <c r="C302">
+        <v>22311546</v>
+      </c>
+      <c r="D302">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="303" spans="1:4">
+      <c r="A303" s="1">
+        <v>301</v>
+      </c>
+      <c r="B303" t="s">
+        <v>304</v>
+      </c>
+      <c r="C303">
+        <v>22430931</v>
+      </c>
+      <c r="D303">
+        <v>0.63</v>
+      </c>
+    </row>
+    <row r="304" spans="1:4">
+      <c r="A304" s="1">
+        <v>302</v>
+      </c>
+      <c r="B304" t="s">
+        <v>305</v>
+      </c>
+      <c r="C304">
+        <v>22465110</v>
+      </c>
+      <c r="D304">
+        <v>0.79</v>
+      </c>
+    </row>
+    <row r="305" spans="1:4">
+      <c r="A305" s="1">
+        <v>303</v>
+      </c>
+      <c r="B305" t="s">
+        <v>306</v>
+      </c>
+      <c r="C305">
+        <v>22417668</v>
+      </c>
+      <c r="D305">
+        <v>0.19</v>
+      </c>
+    </row>
+    <row r="306" spans="1:4">
+      <c r="A306" s="1">
+        <v>304</v>
+      </c>
+      <c r="B306" t="s">
+        <v>307</v>
+      </c>
+      <c r="C306">
         <v>22372044</v>
       </c>
-      <c r="D66">
+      <c r="D306">
         <v>0.1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Arregla seccion asegurados totales, falta el arreglar el corte en los años 2010-11
</commit_message>
<xml_diff>
--- a/data/asegurados_graph1.xlsx
+++ b/data/asegurados_graph1.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="308" uniqueCount="308">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="309" uniqueCount="309">
   <si>
     <t>date_df</t>
   </si>
@@ -938,6 +938,9 @@
   </si>
   <si>
     <t>2025-05-31</t>
+  </si>
+  <si>
+    <t>2025-06-30</t>
   </si>
 </sst>
 </file>
@@ -1295,7 +1298,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D306"/>
+  <dimension ref="A1:D307"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -5546,6 +5549,20 @@
         <v>0.1</v>
       </c>
     </row>
+    <row r="307" spans="1:4">
+      <c r="A307" s="1">
+        <v>305</v>
+      </c>
+      <c r="B307" t="s">
+        <v>308</v>
+      </c>
+      <c r="C307">
+        <v>22325666</v>
+      </c>
+      <c r="D307">
+        <v>0.03</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>